<commit_message>
Added Velocity and Estimates
New and Old Usecases are estimated with the FPs
</commit_message>
<xml_diff>
--- a/TimesSpent.xlsx
+++ b/TimesSpent.xlsx
@@ -5,28 +5,28 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phili\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9195"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="AdministrateBarsFP">Tabelle1!$K$105</definedName>
-    <definedName name="ChangeInfoFP">Tabelle1!$K$81</definedName>
-    <definedName name="CommentFP">Tabelle1!$K$73</definedName>
-    <definedName name="GetBarInfoFP">Tabelle1!$K$57</definedName>
-    <definedName name="LoginFP">Tabelle1!$K$25</definedName>
-    <definedName name="RateBarFP">Tabelle1!$K$65</definedName>
-    <definedName name="RegisterFp">Tabelle1!$K$33</definedName>
-    <definedName name="SearchBarFP">Tabelle1!$K$17</definedName>
-    <definedName name="SeeMapsFP">Tabelle1!$K$89</definedName>
-    <definedName name="SeePinboardsFP">Tabelle1!$K$49</definedName>
-    <definedName name="SetTagsFP">Tabelle1!$K$97</definedName>
-    <definedName name="SurveysFP">Tabelle1!$K$41</definedName>
+    <definedName name="AdministrateBarsFP">Tabelle1!$K$108</definedName>
+    <definedName name="ChangeInfoFP">Tabelle1!$K$84</definedName>
+    <definedName name="CommentFP">Tabelle1!$K$76</definedName>
+    <definedName name="GetBarInfoFP">Tabelle1!$K$60</definedName>
+    <definedName name="LoginFP">Tabelle1!$K$28</definedName>
+    <definedName name="RateBarFP">Tabelle1!$K$68</definedName>
+    <definedName name="RegisterFp">Tabelle1!$K$36</definedName>
+    <definedName name="SearchBarFP">Tabelle1!$K$20</definedName>
+    <definedName name="SeeMapsFP">Tabelle1!$K$92</definedName>
+    <definedName name="SeePinboardsFP">Tabelle1!$K$52</definedName>
+    <definedName name="SetTagsFP">Tabelle1!$K$100</definedName>
+    <definedName name="SurveysFP">Tabelle1!$K$44</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="68">
   <si>
     <t>UC Name</t>
   </si>
@@ -230,6 +230,18 @@
   </si>
   <si>
     <t>CSS with Vaadin, complete recode</t>
+  </si>
+  <si>
+    <t>Velocity</t>
+  </si>
+  <si>
+    <t>Time spent (w/o outliers)</t>
+  </si>
+  <si>
+    <t>Function Points (w/o outliers)</t>
+  </si>
+  <si>
+    <t>Estimate</t>
   </si>
 </sst>
 </file>
@@ -268,20 +280,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="10">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
@@ -297,6 +308,18 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="25" formatCode="hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -430,10 +453,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Tabelle1!$K$3:$K$12</c:f>
+              <c:f>Tabelle1!$L$3:$L$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>11.05</c:v>
                 </c:pt>
@@ -464,15 +487,24 @@
                 <c:pt idx="9">
                   <c:v>28.6</c:v>
                 </c:pt>
+                <c:pt idx="10">
+                  <c:v>20.150000000000002</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11.05</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>16.900000000000002</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Tabelle1!$I$3:$I$12</c:f>
+              <c:f>Tabelle1!$I$3:$I$18</c:f>
               <c:numCache>
                 <c:formatCode>h:mm</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>8.3333333333333301E-2</c:v>
                 </c:pt>
@@ -503,6 +535,15 @@
                 <c:pt idx="9">
                   <c:v>0.27083333333333331</c:v>
                 </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -516,11 +557,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="363054776"/>
-        <c:axId val="363061048"/>
+        <c:axId val="309151616"/>
+        <c:axId val="309155144"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="363054776"/>
+        <c:axId val="309151616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -577,12 +618,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="363061048"/>
+        <c:crossAx val="309155144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="363061048"/>
+        <c:axId val="309155144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -602,7 +643,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="h:mm" sourceLinked="1"/>
+        <c:numFmt formatCode="[h]:mm:ss;@" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -639,9 +680,10 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="363054776"/>
+        <c:crossAx val="309151616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:majorUnit val="2.0833300000000003E-2"/>
       </c:valAx>
       <c:spPr>
         <a:gradFill>
@@ -699,6 +741,7 @@
     <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
+  <c:userShapes r:id="rId1"/>
 </c:chartSpace>
 </file>
 
@@ -706,16 +749,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>4762</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>15875</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>187324</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>80962</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>31749</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -737,25 +780,72 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.08088</cdr:x>
+      <cdr:y>0.11718</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.79289</cdr:x>
+      <cdr:y>0.92978</cdr:y>
+    </cdr:to>
+    <cdr:cxnSp macro="">
+      <cdr:nvCxnSpPr>
+        <cdr:cNvPr id="10" name="Gerader Verbinder 9"/>
+        <cdr:cNvCxnSpPr/>
+      </cdr:nvCxnSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" flipV="1">
+          <a:off x="523875" y="463551"/>
+          <a:ext cx="4611688" cy="3214688"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:style>
+        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </cdr:style>
+    </cdr:cxnSp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="B2:L12" totalsRowShown="0">
-  <autoFilter ref="B2:L12"/>
-  <sortState ref="B3:K12">
-    <sortCondition ref="K2:K12"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="B2:M15" totalsRowShown="0">
+  <autoFilter ref="B2:M15"/>
+  <sortState ref="B3:L12">
+    <sortCondition ref="L2:L12"/>
   </sortState>
-  <tableColumns count="11">
+  <tableColumns count="12">
     <tableColumn id="1" name="UC Name"/>
     <tableColumn id="2" name="Documentation"/>
-    <tableColumn id="7" name="UI Design" dataDxfId="6"/>
-    <tableColumn id="8" name="Database" dataDxfId="5"/>
-    <tableColumn id="9" name="Warmup Phase" dataDxfId="4"/>
+    <tableColumn id="7" name="UI Design" dataDxfId="5"/>
+    <tableColumn id="8" name="Database" dataDxfId="4"/>
+    <tableColumn id="9" name="Warmup Phase" dataDxfId="3"/>
     <tableColumn id="3" name="Coding"/>
     <tableColumn id="4" name="Testing"/>
-    <tableColumn id="10" name="Total w/o warmup" dataDxfId="3">
+    <tableColumn id="10" name="Total w/o warmup" dataDxfId="2">
       <calculatedColumnFormula>SUM(Tabelle1[[#This Row],[Documentation]:[Database]])+SUM(Tabelle1[[#This Row],[Coding]:[Testing]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Total" dataDxfId="2">
+    <tableColumn id="5" name="Total" dataDxfId="1">
       <calculatedColumnFormula>SUM(Tabelle1[[#This Row],[Documentation]:[Testing]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="12" name="Estimate" dataDxfId="0">
+      <calculatedColumnFormula>Tabelle1[[#This Row],[FP]]/Tabelle15[Velocity]/24</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" name="FP"/>
     <tableColumn id="11" name="Explaniation"/>
@@ -765,8 +855,8 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Tabelle10" displayName="Tabelle10" ref="B80:K85" totalsRowShown="0">
-  <autoFilter ref="B80:K85"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Tabelle10" displayName="Tabelle10" ref="B83:K88" totalsRowShown="0">
+  <autoFilter ref="B83:K88"/>
   <tableColumns count="10">
     <tableColumn id="1" name="Change personal information"/>
     <tableColumn id="2" name="Count"/>
@@ -786,8 +876,8 @@
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Tabelle11" displayName="Tabelle11" ref="B88:K93" totalsRowShown="0">
-  <autoFilter ref="B88:K93"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Tabelle11" displayName="Tabelle11" ref="B91:K96" totalsRowShown="0">
+  <autoFilter ref="B91:K96"/>
   <tableColumns count="10">
     <tableColumn id="1" name="See Maps"/>
     <tableColumn id="2" name="Count"/>
@@ -807,8 +897,8 @@
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Tabelle12" displayName="Tabelle12" ref="B96:K101" totalsRowShown="0">
-  <autoFilter ref="B96:K101"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Tabelle12" displayName="Tabelle12" ref="B99:K104" totalsRowShown="0">
+  <autoFilter ref="B99:K104"/>
   <tableColumns count="10">
     <tableColumn id="1" name="Set Tags"/>
     <tableColumn id="2" name="Count"/>
@@ -828,8 +918,8 @@
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Tabelle1214" displayName="Tabelle1214" ref="B104:K109" totalsRowShown="0">
-  <autoFilter ref="B104:K109"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Tabelle1214" displayName="Tabelle1214" ref="B107:K112" totalsRowShown="0">
+  <autoFilter ref="B107:K112"/>
   <tableColumns count="10">
     <tableColumn id="1" name="Administrate Bars"/>
     <tableColumn id="2" name="Count"/>
@@ -849,8 +939,8 @@
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Tabelle121415" displayName="Tabelle121415" ref="B112:K117" totalsRowShown="0">
-  <autoFilter ref="B112:K117"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Tabelle121415" displayName="Tabelle121415" ref="B115:K120" totalsRowShown="0">
+  <autoFilter ref="B115:K120"/>
   <tableColumns count="10">
     <tableColumn id="1" name="Name"/>
     <tableColumn id="2" name="Count"/>
@@ -869,17 +959,35 @@
 </table>
 </file>
 
+<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Tabelle15" displayName="Tabelle15" ref="O23:Q24" totalsRowShown="0">
+  <autoFilter ref="O23:Q24"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Time spent (w/o outliers)" dataDxfId="7">
+      <calculatedColumnFormula>SUM(I3:I10,I12)*24</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="2" name="Function Points (w/o outliers)">
+      <calculatedColumnFormula>SUM(L3:L10,L12)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" name="Velocity" dataDxfId="6">
+      <calculatedColumnFormula>P24/O24</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabelle2" displayName="Tabelle2" ref="B16:K21" totalsRowShown="0">
-  <autoFilter ref="B16:K21"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabelle2" displayName="Tabelle2" ref="B19:K24" totalsRowShown="0">
+  <autoFilter ref="B19:K24"/>
   <tableColumns count="10">
     <tableColumn id="1" name="Search bar"/>
     <tableColumn id="2" name="Count"/>
     <tableColumn id="3" name="Simple"/>
-    <tableColumn id="4" name="Average" dataDxfId="1">
+    <tableColumn id="4" name="Average" dataDxfId="9">
       <calculatedColumnFormula>IF(OR(AND(Tabelle2[[#This Row],[FTR/RET]]=1, Tabelle2[[#This Row],[DET]] &gt; 50), AND(Tabelle2[[#This Row],[FTR/RET]]&lt;=5, Tabelle2[[#This Row],[FTR/RET]]&gt;=2, Tabelle2[[#This Row],[DET]] &gt;= 20, Tabelle2[[#This Row],[DET]] &lt;= 50), AND(Tabelle2[[#This Row],[FTR/RET]] &gt;= 5, Tabelle2[[#This Row],[DET]] &lt; 20)), "x", "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Complex" dataDxfId="0">
+    <tableColumn id="5" name="Complex" dataDxfId="8">
       <calculatedColumnFormula>IF(AND(Tabelle2[[#This Row],[Simple]]="",Tabelle2[[#This Row],[Average]]=""), "x", "")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" name="FTR/RET"/>
@@ -893,8 +1001,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabelle3" displayName="Tabelle3" ref="B24:K29" totalsRowShown="0">
-  <autoFilter ref="B24:K29"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabelle3" displayName="Tabelle3" ref="B27:K32" totalsRowShown="0">
+  <autoFilter ref="B27:K32"/>
   <tableColumns count="10">
     <tableColumn id="1" name="Login"/>
     <tableColumn id="2" name="Count"/>
@@ -914,8 +1022,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabelle4" displayName="Tabelle4" ref="B32:K37" totalsRowShown="0">
-  <autoFilter ref="B32:K37"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabelle4" displayName="Tabelle4" ref="B35:K40" totalsRowShown="0">
+  <autoFilter ref="B35:K40"/>
   <tableColumns count="10">
     <tableColumn id="1" name="Register"/>
     <tableColumn id="2" name="Count"/>
@@ -935,8 +1043,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabelle5" displayName="Tabelle5" ref="B40:K45" totalsRowShown="0">
-  <autoFilter ref="B40:K45"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabelle5" displayName="Tabelle5" ref="B43:K48" totalsRowShown="0">
+  <autoFilter ref="B43:K48"/>
   <tableColumns count="10">
     <tableColumn id="1" name="Surveys"/>
     <tableColumn id="2" name="Count"/>
@@ -956,8 +1064,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabelle6" displayName="Tabelle6" ref="B48:K53" totalsRowShown="0">
-  <autoFilter ref="B48:K53"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabelle6" displayName="Tabelle6" ref="B51:K56" totalsRowShown="0">
+  <autoFilter ref="B51:K56"/>
   <tableColumns count="10">
     <tableColumn id="1" name="See pinboards"/>
     <tableColumn id="2" name="Count"/>
@@ -977,8 +1085,8 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabelle7" displayName="Tabelle7" ref="B56:K61" totalsRowShown="0">
-  <autoFilter ref="B56:K61"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabelle7" displayName="Tabelle7" ref="B59:K64" totalsRowShown="0">
+  <autoFilter ref="B59:K64"/>
   <tableColumns count="10">
     <tableColumn id="1" name="Get bar informations"/>
     <tableColumn id="2" name="Count"/>
@@ -998,8 +1106,8 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tabelle8" displayName="Tabelle8" ref="B64:K69" totalsRowShown="0">
-  <autoFilter ref="B64:K69"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tabelle8" displayName="Tabelle8" ref="B67:K72" totalsRowShown="0">
+  <autoFilter ref="B67:K72"/>
   <tableColumns count="10">
     <tableColumn id="1" name="Rate bar"/>
     <tableColumn id="2" name="Count"/>
@@ -1019,8 +1127,8 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tabelle9" displayName="Tabelle9" ref="B72:K77" totalsRowShown="0">
-  <autoFilter ref="B72:K77"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tabelle9" displayName="Tabelle9" ref="B75:K80" totalsRowShown="0">
+  <autoFilter ref="B75:K80"/>
   <tableColumns count="10">
     <tableColumn id="1" name="Comment at pinboards"/>
     <tableColumn id="2" name="Count"/>
@@ -1303,10 +1411,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="B2:L117"/>
+  <dimension ref="B2:Q120"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1315,9 +1423,11 @@
     <col min="2" max="2" width="28.85546875" customWidth="1"/>
     <col min="3" max="3" width="16.85546875" customWidth="1"/>
     <col min="10" max="10" width="16.85546875" customWidth="1"/>
+    <col min="14" max="14" width="3.28515625" customWidth="1"/>
+    <col min="15" max="15" width="28.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -1346,13 +1456,16 @@
         <v>4</v>
       </c>
       <c r="K2" t="s">
+        <v>67</v>
+      </c>
+      <c r="L2" t="s">
         <v>5</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>13</v>
       </c>
@@ -1382,12 +1495,16 @@
         <f>SUM(Tabelle1[[#This Row],[Documentation]:[Testing]])</f>
         <v>8.3333333333333301E-2</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="2">
+        <f>Tabelle1[[#This Row],[FP]]/Tabelle15[Velocity]/24</f>
+        <v>0.11610422405876951</v>
+      </c>
+      <c r="L3">
         <f>CommentFP</f>
         <v>11.05</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>10</v>
       </c>
@@ -1417,12 +1534,16 @@
         <f>SUM(Tabelle1[[#This Row],[Documentation]:[Testing]])</f>
         <v>0.13194444444444445</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="2">
+        <f>Tabelle1[[#This Row],[FP]]/Tabelle15[Velocity]/24</f>
+        <v>0.14342286501377408</v>
+      </c>
+      <c r="L4">
         <f>SeePinboardsFP</f>
         <v>13.65</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>7</v>
       </c>
@@ -1452,12 +1573,16 @@
         <f>SUM(Tabelle1[[#This Row],[Documentation]:[Testing]])</f>
         <v>0.3125</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="2">
+        <f>Tabelle1[[#This Row],[FP]]/Tabelle15[Velocity]/24</f>
+        <v>0.16391184573002754</v>
+      </c>
+      <c r="L5">
         <f>LoginFP</f>
         <v>15.600000000000001</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>12</v>
       </c>
@@ -1487,15 +1612,19 @@
         <f>SUM(Tabelle1[[#This Row],[Documentation]:[Testing]])</f>
         <v>0.32638888888888884</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="2">
+        <f>Tabelle1[[#This Row],[FP]]/Tabelle15[Velocity]/24</f>
+        <v>0.18387546796637702</v>
+      </c>
+      <c r="L6">
         <f>RateBarFP</f>
         <v>17.5</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>6</v>
       </c>
@@ -1525,12 +1654,16 @@
         <f>SUM(Tabelle1[[#This Row],[Documentation]:[Testing]])</f>
         <v>0.15277777777777779</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="2">
+        <f>Tabelle1[[#This Row],[FP]]/Tabelle15[Velocity]/24</f>
+        <v>0.14342286501377408</v>
+      </c>
+      <c r="L7">
         <f>SearchBarFP</f>
         <v>13.65</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>11</v>
       </c>
@@ -1560,12 +1693,16 @@
         <f>SUM(Tabelle1[[#This Row],[Documentation]:[Testing]])</f>
         <v>0.17361111111111105</v>
       </c>
-      <c r="K8">
+      <c r="K8" s="2">
+        <f>Tabelle1[[#This Row],[FP]]/Tabelle15[Velocity]/24</f>
+        <v>0.19123048668503209</v>
+      </c>
+      <c r="L8">
         <f>GetBarInfoFP</f>
         <v>18.2</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>9</v>
       </c>
@@ -1595,12 +1732,16 @@
         <f>SUM(Tabelle1[[#This Row],[Documentation]:[Testing]])</f>
         <v>0.20138888888888887</v>
       </c>
-      <c r="K9">
+      <c r="K9" s="2">
+        <f>Tabelle1[[#This Row],[FP]]/Tabelle15[Velocity]/24</f>
+        <v>0.19858550540368722</v>
+      </c>
+      <c r="L9">
         <f>SurveysFP</f>
         <v>18.900000000000002</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>43</v>
       </c>
@@ -1630,12 +1771,16 @@
         <f>SUM(Tabelle1[[#This Row],[Documentation]:[Testing]])</f>
         <v>0.3125</v>
       </c>
-      <c r="K10">
+      <c r="K10" s="2">
+        <f>Tabelle1[[#This Row],[FP]]/Tabelle15[Velocity]/24</f>
+        <v>0.21171946740128558</v>
+      </c>
+      <c r="L10">
         <f>SeeMapsFP</f>
         <v>20.150000000000002</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>14</v>
       </c>
@@ -1665,15 +1810,19 @@
         <f>SUM(Tabelle1[[#This Row],[Documentation]:[Testing]])</f>
         <v>0.15277777777777773</v>
       </c>
-      <c r="K11">
+      <c r="K11" s="2">
+        <f>Tabelle1[[#This Row],[FP]]/Tabelle15[Velocity]/24</f>
+        <v>0.30050505050505044</v>
+      </c>
+      <c r="L11">
         <f>ChangeInfoFP</f>
         <v>28.6</v>
       </c>
-      <c r="L11" t="s">
+      <c r="M11" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>8</v>
       </c>
@@ -1703,2465 +1852,2491 @@
         <f>SUM(Tabelle1[[#This Row],[Documentation]:[Testing]])</f>
         <v>0.35416666666666663</v>
       </c>
-      <c r="K12">
+      <c r="K12" s="2">
+        <f>Tabelle1[[#This Row],[FP]]/Tabelle15[Velocity]/24</f>
+        <v>0.30050505050505044</v>
+      </c>
+      <c r="L12">
         <f>RegisterFp</f>
         <v>28.6</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>43</v>
+      </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="2"/>
-    </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="I13" s="1">
+        <f>SUM(Tabelle1[[#This Row],[Documentation]:[Database]])+SUM(Tabelle1[[#This Row],[Coding]:[Testing]])</f>
+        <v>0</v>
+      </c>
+      <c r="J13" s="2">
+        <f>SUM(Tabelle1[[#This Row],[Documentation]:[Testing]])</f>
+        <v>0</v>
+      </c>
+      <c r="K13" s="2">
+        <f>Tabelle1[[#This Row],[FP]]/Tabelle15[Velocity]/24</f>
+        <v>0.21171946740128558</v>
+      </c>
+      <c r="L13">
+        <f>SeeMapsFP</f>
+        <v>20.150000000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>45</v>
+      </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="2"/>
-    </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
+      <c r="I14" s="1">
+        <f>SUM(Tabelle1[[#This Row],[Documentation]:[Database]])+SUM(Tabelle1[[#This Row],[Coding]:[Testing]])</f>
+        <v>0</v>
+      </c>
+      <c r="J14" s="2">
+        <f>SUM(Tabelle1[[#This Row],[Documentation]:[Testing]])</f>
+        <v>0</v>
+      </c>
+      <c r="K14" s="2">
+        <f>Tabelle1[[#This Row],[FP]]/Tabelle15[Velocity]/24</f>
+        <v>0.11610422405876951</v>
+      </c>
+      <c r="L14">
+        <f>SetTagsFP</f>
+        <v>11.05</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1">
+        <f>SUM(Tabelle1[[#This Row],[Documentation]:[Database]])+SUM(Tabelle1[[#This Row],[Coding]:[Testing]])</f>
+        <v>0</v>
+      </c>
+      <c r="J15" s="2">
+        <f>SUM(Tabelle1[[#This Row],[Documentation]:[Testing]])</f>
+        <v>0</v>
+      </c>
+      <c r="K15" s="2">
+        <f>Tabelle1[[#This Row],[FP]]/Tabelle15[Velocity]/24</f>
+        <v>0.17757116620752986</v>
+      </c>
+      <c r="L15">
+        <f>AdministrateBarsFP</f>
+        <v>16.900000000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="4"/>
+    </row>
+    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="4"/>
+    </row>
+    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
         <v>17</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C19" t="s">
         <v>21</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D19" t="s">
         <v>18</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E19" t="s">
         <v>19</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F19" t="s">
         <v>20</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G19" t="s">
         <v>49</v>
       </c>
-      <c r="H16" t="s">
+      <c r="H19" t="s">
         <v>29</v>
       </c>
-      <c r="I16" t="s">
+      <c r="I19" t="s">
         <v>50</v>
       </c>
-      <c r="J16" t="s">
+      <c r="J19" t="s">
         <v>22</v>
       </c>
-      <c r="K16" t="s">
+      <c r="K19" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
         <v>24</v>
       </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-      <c r="D17">
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
         <f>IF(OR(AND(Tabelle2[[#This Row],[FTR/RET]]&lt;=1, Tabelle2[[#This Row],[DET]] &lt;= 15), AND(Tabelle2[[#This Row],[FTR/RET]]&lt;= 3, Tabelle2[[#This Row],[DET]] &lt;= 4)), 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="E17">
+      <c r="E20">
         <f>IF(OR(AND(Tabelle2[[#This Row],[FTR/RET]]&lt;=1, Tabelle2[[#This Row],[DET]] &gt; 15), AND(Tabelle2[[#This Row],[FTR/RET]]&lt;=5, Tabelle2[[#This Row],[FTR/RET]]&gt;=2, Tabelle2[[#This Row],[DET]] &gt;= 5, Tabelle2[[#This Row],[DET]] &lt;= 15), AND(Tabelle2[[#This Row],[FTR/RET]] &gt;= 5, Tabelle2[[#This Row],[DET]] &lt;= 4 )), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="F17">
+      <c r="F20">
         <f>IF(AND(Tabelle2[[#This Row],[Simple]]=0,Tabelle2[[#This Row],[Average]]=0), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="G17">
-        <v>0</v>
-      </c>
-      <c r="H17">
-        <v>0</v>
-      </c>
-      <c r="I17">
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
         <f>Tabelle2[[#This Row],[Count]]*(3*Tabelle2[[#This Row],[Simple]]+4*Tabelle2[[#This Row],[Average]]+6*Tabelle2[[#This Row],[Complex]])</f>
         <v>0</v>
       </c>
-      <c r="J17" t="s">
+      <c r="J20" t="s">
         <v>23</v>
       </c>
-      <c r="K17">
+      <c r="K20">
         <f>SUM(Tabelle2[Points])*0.65</f>
         <v>13.65</v>
       </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
+    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
         <v>25</v>
       </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
-      <c r="D18">
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
         <f>IF(OR(AND(Tabelle2[[#This Row],[FTR/RET]]&lt;=1, Tabelle2[[#This Row],[DET]] &lt;= 19), AND(Tabelle2[[#This Row],[FTR/RET]]&lt;= 3, Tabelle2[[#This Row],[DET]] &lt;= 5)), 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="E18">
+      <c r="E21">
         <f>IF(OR(AND(Tabelle2[[#This Row],[FTR/RET]]&lt;=1, Tabelle2[[#This Row],[DET]] &gt; 20), AND(Tabelle2[[#This Row],[FTR/RET]]&lt;=5, Tabelle2[[#This Row],[FTR/RET]]&gt;=2, Tabelle2[[#This Row],[DET]] &gt;= 6, Tabelle2[[#This Row],[DET]] &lt;= 19), AND(Tabelle2[[#This Row],[FTR/RET]] &gt;= 5, Tabelle2[[#This Row],[DET]] &lt;= 5 )), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="F18">
+      <c r="F21">
         <f>IF(AND(Tabelle2[[#This Row],[Simple]]=0,Tabelle2[[#This Row],[Average]]=0), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="G18">
-        <v>0</v>
-      </c>
-      <c r="H18">
-        <v>1</v>
-      </c>
-      <c r="I18">
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="I21">
         <f>Tabelle2[[#This Row],[Count]]*(Tabelle2[[#This Row],[Simple]]*4+Tabelle2[[#This Row],[Average]]*5+Tabelle2[[#This Row],[Complex]]*7)</f>
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
+    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
         <v>26</v>
       </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
-      <c r="D19">
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
         <f>IF(OR(AND(Tabelle2[[#This Row],[FTR/RET]]&lt;=1, Tabelle2[[#This Row],[DET]] &lt;= 19), AND(Tabelle2[[#This Row],[FTR/RET]]&lt;= 3, Tabelle2[[#This Row],[DET]] &lt;= 5)), 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="E19">
+      <c r="E22">
         <f>IF(OR(AND(Tabelle2[[#This Row],[FTR/RET]]&lt;=1, Tabelle2[[#This Row],[DET]] &gt; 20), AND(Tabelle2[[#This Row],[FTR/RET]]&lt;=5, Tabelle2[[#This Row],[FTR/RET]]&gt;=2, Tabelle2[[#This Row],[DET]] &gt;= 6, Tabelle2[[#This Row],[DET]] &lt;= 19), AND(Tabelle2[[#This Row],[FTR/RET]] &gt;= 5, Tabelle2[[#This Row],[DET]] &lt;= 5 )), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="F19">
+      <c r="F22">
         <f>IF(AND(Tabelle2[[#This Row],[Simple]]=0,Tabelle2[[#This Row],[Average]]=0), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="G19">
-        <v>0</v>
-      </c>
-      <c r="H19">
-        <v>1</v>
-      </c>
-      <c r="I19">
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22">
         <f>Tabelle2[[#This Row],[Count]]*(3*Tabelle2[[#This Row],[Simple]]+4*Tabelle2[[#This Row],[Average]]+6*Tabelle2[[#This Row],[Complex]])</f>
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
+    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
         <v>27</v>
       </c>
-      <c r="C20">
+      <c r="C23">
         <v>2</v>
       </c>
-      <c r="D20">
+      <c r="D23">
         <f>IF(OR(AND(Tabelle2[[#This Row],[FTR/RET]]&lt;2, Tabelle2[[#This Row],[DET]] &lt;= 50), AND(Tabelle2[[#This Row],[FTR/RET]]&lt;=5, Tabelle2[[#This Row],[DET]] &lt; 20)), 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="E20">
+      <c r="E23">
         <f>IF(OR(AND(Tabelle2[[#This Row],[FTR/RET]]=1, Tabelle2[[#This Row],[DET]] &gt; 50), AND(Tabelle2[[#This Row],[FTR/RET]]&lt;=5, Tabelle2[[#This Row],[FTR/RET]]&gt;=2, Tabelle2[[#This Row],[DET]] &gt;= 20, Tabelle2[[#This Row],[DET]] &lt;= 50), AND(Tabelle2[[#This Row],[FTR/RET]] &gt;= 5, Tabelle2[[#This Row],[DET]] &lt; 20)), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="F20">
+      <c r="F23">
         <f>IF(AND(Tabelle2[[#This Row],[Simple]]=0,Tabelle2[[#This Row],[Average]]=0), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="G20">
-        <v>0</v>
-      </c>
-      <c r="H20">
-        <v>1</v>
-      </c>
-      <c r="I20">
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="I23">
         <f>Tabelle2[[#This Row],[Count]]*(7*Tabelle2[[#This Row],[Simple]]+10*Tabelle2[[#This Row],[Average]]+15*Tabelle2[[#This Row],[Complex]])</f>
         <v>14</v>
       </c>
-      <c r="J20" t="s">
+      <c r="J23" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
+      <c r="O23" t="s">
+        <v>65</v>
+      </c>
+      <c r="P23" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
         <v>28</v>
       </c>
-      <c r="C21">
-        <v>0</v>
-      </c>
-      <c r="D21">
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
         <f>IF(OR(AND(Tabelle2[[#This Row],[FTR/RET]]&lt;2, Tabelle2[[#This Row],[DET]] &lt;= 50), AND(Tabelle2[[#This Row],[FTR/RET]]&lt;=5, Tabelle2[[#This Row],[DET]] &lt; 20)), 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="E21">
+      <c r="E24">
         <f>IF(OR(AND(Tabelle2[[#This Row],[FTR/RET]]=1, Tabelle2[[#This Row],[DET]] &gt; 50), AND(Tabelle2[[#This Row],[FTR/RET]]&lt;=5, Tabelle2[[#This Row],[FTR/RET]]&gt;=2, Tabelle2[[#This Row],[DET]] &gt;= 20, Tabelle2[[#This Row],[DET]] &lt;= 50), AND(Tabelle2[[#This Row],[FTR/RET]] &gt;= 5, Tabelle2[[#This Row],[DET]] &lt; 20)), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="F21">
+      <c r="F24">
         <f>IF(AND(Tabelle2[[#This Row],[Simple]]=0,Tabelle2[[#This Row],[Average]]=0), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="G21">
-        <v>0</v>
-      </c>
-      <c r="H21">
-        <v>0</v>
-      </c>
-      <c r="I21">
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
         <f>Tabelle2[[#This Row],[Count]]*(5*Tabelle2[[#This Row],[Simple]]+7*Tabelle2[[#This Row],[Average]]+10*Tabelle2[[#This Row],[Complex]])</f>
         <v>0</v>
       </c>
-      <c r="J21" t="s">
+      <c r="J24" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
+      <c r="O24" s="4">
+        <f>SUM(I3:I10,I12)*24</f>
+        <v>39.666666666666664</v>
+      </c>
+      <c r="P24">
+        <f>SUM(L3:L10,L12)</f>
+        <v>157.30000000000001</v>
+      </c>
+      <c r="Q24" s="3">
+        <f>P24/O24</f>
+        <v>3.9655462184873955</v>
+      </c>
+    </row>
+    <row r="27" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
         <v>7</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C27" t="s">
         <v>21</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D27" t="s">
         <v>18</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E27" t="s">
         <v>19</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F27" t="s">
         <v>20</v>
       </c>
-      <c r="G24" t="s">
+      <c r="G27" t="s">
         <v>49</v>
       </c>
-      <c r="H24" t="s">
+      <c r="H27" t="s">
         <v>29</v>
       </c>
-      <c r="I24" t="s">
+      <c r="I27" t="s">
         <v>50</v>
       </c>
-      <c r="J24" t="s">
+      <c r="J27" t="s">
         <v>22</v>
       </c>
-      <c r="K24" t="s">
+      <c r="K27" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
+    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
         <v>24</v>
       </c>
-      <c r="C25">
-        <v>0</v>
-      </c>
-      <c r="D25">
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
         <f>IF(OR(AND(Tabelle3[[#This Row],[FTR/RET]]&lt;=1,Tabelle3[[#This Row],[DET]] &lt;= 15), AND(Tabelle3[[#This Row],[FTR/RET]]&lt;= 3,Tabelle3[[#This Row],[DET]] &lt;= 4)), 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="E25">
+      <c r="E28">
         <f>IF(OR(AND(Tabelle3[[#This Row],[FTR/RET]]&lt;=1, Tabelle3[[#This Row],[DET]] &gt; 15), AND(Tabelle3[[#This Row],[FTR/RET]]&lt;=5, Tabelle3[[#This Row],[FTR/RET]]&gt;=2, Tabelle3[[#This Row],[DET]] &gt;= 5, Tabelle3[[#This Row],[DET]] &lt;= 15), AND(Tabelle3[[#This Row],[FTR/RET]] &gt;= 5, Tabelle3[[#This Row],[DET]] &lt;= 4 )), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="F25">
+      <c r="F28">
         <f>IF(AND(Tabelle3[[#This Row],[Simple]]=0,Tabelle3[[#This Row],[Average]]=0), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="G25">
-        <v>0</v>
-      </c>
-      <c r="H25">
-        <v>0</v>
-      </c>
-      <c r="I25">
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28">
         <f>Tabelle3[[#This Row],[Count]]*(3*Tabelle3[[#This Row],[Simple]]+4*Tabelle3[[#This Row],[Average]]+6*Tabelle3[[#This Row],[Complex]])</f>
         <v>0</v>
       </c>
-      <c r="J25" t="s">
+      <c r="J28" t="s">
         <v>33</v>
       </c>
-      <c r="K25">
+      <c r="K28">
         <f>SUM(Tabelle3[Points])*0.65</f>
         <v>15.600000000000001</v>
       </c>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
+    <row r="29" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
         <v>25</v>
       </c>
-      <c r="C26">
-        <v>0</v>
-      </c>
-      <c r="D26">
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
         <f>IF(OR(AND(Tabelle3[[#This Row],[FTR/RET]]&lt;=1, Tabelle3[[#This Row],[DET]] &lt;= 19), AND(Tabelle3[[#This Row],[FTR/RET]]&lt;= 3, Tabelle3[[#This Row],[DET]] &lt;= 5)), 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="E26">
+      <c r="E29">
         <f>IF(OR(AND(Tabelle3[[#This Row],[FTR/RET]]&lt;=1, Tabelle3[[#This Row],[DET]] &gt; 20), AND(Tabelle3[[#This Row],[FTR/RET]]&lt;=5, Tabelle3[[#This Row],[FTR/RET]]&gt;=2, Tabelle3[[#This Row],[DET]] &gt;= 6, Tabelle3[[#This Row],[DET]] &lt;= 19), AND(Tabelle3[[#This Row],[FTR/RET]] &gt;= 5, Tabelle3[[#This Row],[DET]] &lt;= 5 )), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="F26">
+      <c r="F29">
         <f>IF(AND(Tabelle3[[#This Row],[Simple]]=0,Tabelle3[[#This Row],[Average]]=0), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="G26">
-        <v>0</v>
-      </c>
-      <c r="H26">
-        <v>0</v>
-      </c>
-      <c r="I26">
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
         <f>Tabelle3[[#This Row],[Count]]*(Tabelle3[[#This Row],[Simple]]*4+Tabelle3[[#This Row],[Average]]*5+Tabelle3[[#This Row],[Complex]]*7)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
+    <row r="30" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
         <v>26</v>
       </c>
-      <c r="C27">
-        <v>1</v>
-      </c>
-      <c r="D27">
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30">
         <f>IF(OR(AND(Tabelle3[[#This Row],[FTR/RET]]&lt;=1, Tabelle3[[#This Row],[DET]] &lt;= 19), AND(Tabelle3[[#This Row],[FTR/RET]]&lt;= 3, Tabelle3[[#This Row],[DET]] &lt;= 5)), 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="E27">
+      <c r="E30">
         <f>IF(OR(AND(Tabelle3[[#This Row],[FTR/RET]]&lt;=1, Tabelle3[[#This Row],[DET]] &gt; 20), AND(Tabelle3[[#This Row],[FTR/RET]]&lt;=5, Tabelle3[[#This Row],[FTR/RET]]&gt;=2, Tabelle3[[#This Row],[DET]] &gt;= 6, Tabelle3[[#This Row],[DET]] &lt;= 19), AND(Tabelle3[[#This Row],[FTR/RET]] &gt;= 5, Tabelle3[[#This Row],[DET]] &lt;= 5 )), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="F27">
+      <c r="F30">
         <f>IF(AND(Tabelle3[[#This Row],[Simple]]=0,Tabelle3[[#This Row],[Average]]=0), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="G27">
-        <v>0</v>
-      </c>
-      <c r="H27">
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30">
         <v>2</v>
       </c>
-      <c r="I27">
+      <c r="I30">
         <f>Tabelle3[[#This Row],[Count]]*(3*Tabelle3[[#This Row],[Simple]]+4*Tabelle3[[#This Row],[Average]]+6*Tabelle3[[#This Row],[Complex]])</f>
         <v>3</v>
       </c>
-      <c r="J27" t="s">
+      <c r="J30" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
+    <row r="31" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
         <v>27</v>
       </c>
-      <c r="C28">
+      <c r="C31">
         <v>3</v>
       </c>
-      <c r="D28">
+      <c r="D31">
         <f>IF(OR(AND(Tabelle3[[#This Row],[FTR/RET]]&lt;2, Tabelle3[[#This Row],[DET]] &lt;= 50), AND(Tabelle3[[#This Row],[FTR/RET]]&lt;=5, Tabelle3[[#This Row],[DET]] &lt; 20)), 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="E28">
+      <c r="E31">
         <f>IF(OR(AND(Tabelle3[[#This Row],[FTR/RET]]=1, Tabelle3[[#This Row],[DET]] &gt; 50), AND(Tabelle3[[#This Row],[FTR/RET]]&lt;=5, Tabelle3[[#This Row],[FTR/RET]]&gt;=2, Tabelle3[[#This Row],[DET]] &gt;= 20, Tabelle3[[#This Row],[DET]] &lt;= 50), AND(Tabelle3[[#This Row],[FTR/RET]] &gt;= 5, Tabelle3[[#This Row],[DET]] &lt; 20)), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="F28">
+      <c r="F31">
         <f>IF(AND(Tabelle3[[#This Row],[Simple]]=0,Tabelle3[[#This Row],[Average]]=0), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="G28">
-        <v>0</v>
-      </c>
-      <c r="H28">
-        <v>0</v>
-      </c>
-      <c r="I28">
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31">
         <f>Tabelle3[[#This Row],[Count]]*(7*Tabelle3[[#This Row],[Simple]]+10*Tabelle3[[#This Row],[Average]]+15*Tabelle3[[#This Row],[Complex]])</f>
         <v>21</v>
       </c>
-      <c r="J28" t="s">
+      <c r="J31" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
+    <row r="32" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
         <v>28</v>
       </c>
-      <c r="C29">
-        <v>0</v>
-      </c>
-      <c r="D29">
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
         <f>IF(OR(AND(Tabelle3[[#This Row],[FTR/RET]]&lt;2, Tabelle3[[#This Row],[DET]] &lt;= 50), AND(Tabelle3[[#This Row],[FTR/RET]]&lt;=5, Tabelle3[[#This Row],[DET]] &lt; 20)), 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="E29">
+      <c r="E32">
         <f>IF(OR(AND(Tabelle3[[#This Row],[FTR/RET]]=1, Tabelle3[[#This Row],[DET]] &gt; 50), AND(Tabelle3[[#This Row],[FTR/RET]]&lt;=5, Tabelle3[[#This Row],[FTR/RET]]&gt;=2, Tabelle3[[#This Row],[DET]] &gt;= 20, Tabelle3[[#This Row],[DET]] &lt;= 50), AND(Tabelle3[[#This Row],[FTR/RET]] &gt;= 5, Tabelle3[[#This Row],[DET]] &lt; 20)), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="F29">
+      <c r="F32">
         <f>IF(AND(Tabelle3[[#This Row],[Simple]]=0,Tabelle3[[#This Row],[Average]]=0), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="G29">
-        <v>0</v>
-      </c>
-      <c r="H29">
-        <v>0</v>
-      </c>
-      <c r="I29">
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32">
         <f>Tabelle3[[#This Row],[Count]]*(5*Tabelle3[[#This Row],[Simple]]+7*Tabelle3[[#This Row],[Average]]+10*Tabelle3[[#This Row],[Complex]])</f>
         <v>0</v>
       </c>
-      <c r="J29" t="s">
+      <c r="J32" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
+    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
         <v>8</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C35" t="s">
         <v>21</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D35" t="s">
         <v>18</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E35" t="s">
         <v>19</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F35" t="s">
         <v>20</v>
       </c>
-      <c r="G32" t="s">
+      <c r="G35" t="s">
         <v>49</v>
       </c>
-      <c r="H32" t="s">
+      <c r="H35" t="s">
         <v>29</v>
       </c>
-      <c r="I32" t="s">
+      <c r="I35" t="s">
         <v>50</v>
       </c>
-      <c r="J32" t="s">
+      <c r="J35" t="s">
         <v>22</v>
       </c>
-      <c r="K32" t="s">
+      <c r="K35" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
+    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
         <v>24</v>
       </c>
-      <c r="C33">
+      <c r="C36">
         <v>10</v>
       </c>
-      <c r="D33">
+      <c r="D36">
         <f>IF(OR(AND(Tabelle4[[#This Row],[FTR/RET]]&lt;=1, Tabelle4[[#This Row],[DET]] &lt;= 15), AND(Tabelle4[[#This Row],[FTR/RET]]&lt;= 3, Tabelle4[[#This Row],[DET]] &lt;= 4)), 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="E33">
+      <c r="E36">
         <f>IF(OR(AND(Tabelle4[[#This Row],[FTR/RET]]&lt;=1, Tabelle4[[#This Row],[DET]] &gt; 15), AND(Tabelle4[[#This Row],[FTR/RET]]&lt;=5, Tabelle4[[#This Row],[FTR/RET]]&gt;=2, Tabelle4[[#This Row],[DET]] &gt;= 5, Tabelle4[[#This Row],[DET]] &lt;= 15), AND(Tabelle4[[#This Row],[FTR/RET]] &gt;= 5, Tabelle4[[#This Row],[DET]] &lt;= 4 )), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="F33">
+      <c r="F36">
         <f>IF(AND(Tabelle4[[#This Row],[Simple]]=0,Tabelle4[[#This Row],[Average]]=0), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="G33">
-        <v>1</v>
-      </c>
-      <c r="H33">
+      <c r="G36">
+        <v>1</v>
+      </c>
+      <c r="H36">
         <v>10</v>
       </c>
-      <c r="I33">
+      <c r="I36">
         <f>Tabelle4[[#This Row],[Count]]*(3*Tabelle4[[#This Row],[Simple]]+4*Tabelle4[[#This Row],[Average]]+6*Tabelle4[[#This Row],[Complex]])</f>
         <v>30</v>
       </c>
-      <c r="J33" t="s">
+      <c r="J36" t="s">
         <v>37</v>
       </c>
-      <c r="K33">
+      <c r="K36">
         <f>SUM(Tabelle4[Points])*0.65</f>
         <v>28.6</v>
       </c>
     </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
+    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
         <v>25</v>
       </c>
-      <c r="C34">
-        <v>0</v>
-      </c>
-      <c r="D34">
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
         <f>IF(OR(AND(Tabelle4[[#This Row],[FTR/RET]]&lt;=1, Tabelle4[[#This Row],[DET]] &lt;= 19), AND(Tabelle4[[#This Row],[FTR/RET]]&lt;= 3, Tabelle4[[#This Row],[DET]] &lt;= 5)), 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="E34">
+      <c r="E37">
         <f>IF(OR(AND(Tabelle4[[#This Row],[FTR/RET]]&lt;=1, Tabelle4[[#This Row],[DET]] &gt; 20), AND(Tabelle4[[#This Row],[FTR/RET]]&lt;=5, Tabelle4[[#This Row],[FTR/RET]]&gt;=2, Tabelle4[[#This Row],[DET]] &gt;= 6, Tabelle4[[#This Row],[DET]] &lt;= 19), AND(Tabelle4[[#This Row],[FTR/RET]] &gt;= 5, Tabelle4[[#This Row],[DET]] &lt;= 5 )), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="F34">
+      <c r="F37">
         <f>IF(AND(Tabelle4[[#This Row],[Simple]]=0,Tabelle4[[#This Row],[Average]]=0), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="G34">
-        <v>0</v>
-      </c>
-      <c r="H34">
-        <v>0</v>
-      </c>
-      <c r="I34">
+      <c r="G37">
+        <v>0</v>
+      </c>
+      <c r="H37">
+        <v>0</v>
+      </c>
+      <c r="I37">
         <f>Tabelle4[[#This Row],[Count]]*(Tabelle4[[#This Row],[Simple]]*4+Tabelle4[[#This Row],[Average]]*5+Tabelle4[[#This Row],[Complex]]*7)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
+    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
         <v>26</v>
       </c>
-      <c r="C35">
-        <v>0</v>
-      </c>
-      <c r="D35">
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38">
         <f>IF(OR(AND(Tabelle4[[#This Row],[FTR/RET]]&lt;=1, Tabelle4[[#This Row],[DET]] &lt;= 19), AND(Tabelle4[[#This Row],[FTR/RET]]&lt;= 3, Tabelle4[[#This Row],[DET]] &lt;= 5)), 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="E35">
+      <c r="E38">
         <f>IF(OR(AND(Tabelle4[[#This Row],[FTR/RET]]&lt;=1, Tabelle4[[#This Row],[DET]] &gt; 20), AND(Tabelle4[[#This Row],[FTR/RET]]&lt;=5, Tabelle4[[#This Row],[FTR/RET]]&gt;=2, Tabelle4[[#This Row],[DET]] &gt;= 6, Tabelle4[[#This Row],[DET]] &lt;= 19), AND(Tabelle4[[#This Row],[FTR/RET]] &gt;= 5, Tabelle4[[#This Row],[DET]] &lt;= 5 )), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="F35">
+      <c r="F38">
         <f>IF(AND(Tabelle4[[#This Row],[Simple]]=0,Tabelle4[[#This Row],[Average]]=0), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="G35">
-        <v>0</v>
-      </c>
-      <c r="H35">
-        <v>0</v>
-      </c>
-      <c r="I35">
+      <c r="G38">
+        <v>0</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
+      <c r="I38">
         <f>Tabelle4[[#This Row],[Count]]*(3*Tabelle4[[#This Row],[Simple]]+4*Tabelle4[[#This Row],[Average]]+6*Tabelle4[[#This Row],[Complex]])</f>
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
+    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
         <v>27</v>
       </c>
-      <c r="C36">
+      <c r="C39">
         <v>2</v>
       </c>
-      <c r="D36">
+      <c r="D39">
         <f>IF(OR(AND(Tabelle4[[#This Row],[FTR/RET]]&lt;2, Tabelle4[[#This Row],[DET]] &lt;= 50), AND(Tabelle4[[#This Row],[FTR/RET]]&lt;=5, Tabelle4[[#This Row],[DET]] &lt; 20)), 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="E36">
+      <c r="E39">
         <f>IF(OR(AND(Tabelle4[[#This Row],[FTR/RET]]=1, Tabelle4[[#This Row],[DET]] &gt; 50), AND(Tabelle4[[#This Row],[FTR/RET]]&lt;=5, Tabelle4[[#This Row],[FTR/RET]]&gt;=2, Tabelle4[[#This Row],[DET]] &gt;= 20, Tabelle4[[#This Row],[DET]] &lt;= 50), AND(Tabelle4[[#This Row],[FTR/RET]] &gt;= 5, Tabelle4[[#This Row],[DET]] &lt; 20)), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="F36">
+      <c r="F39">
         <f>IF(AND(Tabelle4[[#This Row],[Simple]]=0,Tabelle4[[#This Row],[Average]]=0), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="G36">
-        <v>1</v>
-      </c>
-      <c r="H36">
+      <c r="G39">
+        <v>1</v>
+      </c>
+      <c r="H39">
         <v>10</v>
       </c>
-      <c r="I36">
+      <c r="I39">
         <f>Tabelle4[[#This Row],[Count]]*(7*Tabelle4[[#This Row],[Simple]]+10*Tabelle4[[#This Row],[Average]]+15*Tabelle4[[#This Row],[Complex]])</f>
         <v>14</v>
       </c>
-      <c r="J36" t="s">
+      <c r="J39" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
-        <v>28</v>
-      </c>
-      <c r="C37">
-        <v>0</v>
-      </c>
-      <c r="D37">
-        <f>IF(OR(AND(Tabelle4[[#This Row],[FTR/RET]]&lt;2, Tabelle4[[#This Row],[DET]] &lt;= 50), AND(Tabelle4[[#This Row],[FTR/RET]]&lt;=5, Tabelle4[[#This Row],[DET]] &lt; 20)), 1, 0)</f>
-        <v>1</v>
-      </c>
-      <c r="E37">
-        <f>IF(OR(AND(Tabelle4[[#This Row],[FTR/RET]]=1, Tabelle4[[#This Row],[DET]] &gt; 50), AND(Tabelle4[[#This Row],[FTR/RET]]&lt;=5, Tabelle4[[#This Row],[FTR/RET]]&gt;=2, Tabelle4[[#This Row],[DET]] &gt;= 20, Tabelle4[[#This Row],[DET]] &lt;= 50), AND(Tabelle4[[#This Row],[FTR/RET]] &gt;= 5, Tabelle4[[#This Row],[DET]] &lt; 20)), 1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="F37">
-        <f>IF(AND(Tabelle4[[#This Row],[Simple]]=0,Tabelle4[[#This Row],[Average]]=0), 1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="G37">
-        <v>0</v>
-      </c>
-      <c r="H37">
-        <v>0</v>
-      </c>
-      <c r="I37">
-        <f>Tabelle4[[#This Row],[Count]]*(5*Tabelle4[[#This Row],[Simple]]+7*Tabelle4[[#This Row],[Average]]+10*Tabelle4[[#This Row],[Complex]])</f>
-        <v>0</v>
       </c>
     </row>
     <row r="40" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
+        <v>28</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="D40">
+        <f>IF(OR(AND(Tabelle4[[#This Row],[FTR/RET]]&lt;2, Tabelle4[[#This Row],[DET]] &lt;= 50), AND(Tabelle4[[#This Row],[FTR/RET]]&lt;=5, Tabelle4[[#This Row],[DET]] &lt; 20)), 1, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="E40">
+        <f>IF(OR(AND(Tabelle4[[#This Row],[FTR/RET]]=1, Tabelle4[[#This Row],[DET]] &gt; 50), AND(Tabelle4[[#This Row],[FTR/RET]]&lt;=5, Tabelle4[[#This Row],[FTR/RET]]&gt;=2, Tabelle4[[#This Row],[DET]] &gt;= 20, Tabelle4[[#This Row],[DET]] &lt;= 50), AND(Tabelle4[[#This Row],[FTR/RET]] &gt;= 5, Tabelle4[[#This Row],[DET]] &lt; 20)), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <f>IF(AND(Tabelle4[[#This Row],[Simple]]=0,Tabelle4[[#This Row],[Average]]=0), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
+      <c r="I40">
+        <f>Tabelle4[[#This Row],[Count]]*(5*Tabelle4[[#This Row],[Simple]]+7*Tabelle4[[#This Row],[Average]]+10*Tabelle4[[#This Row],[Complex]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
         <v>9</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C43" t="s">
         <v>21</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D43" t="s">
         <v>18</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E43" t="s">
         <v>19</v>
       </c>
-      <c r="F40" t="s">
+      <c r="F43" t="s">
         <v>20</v>
       </c>
-      <c r="G40" t="s">
+      <c r="G43" t="s">
         <v>49</v>
       </c>
-      <c r="H40" t="s">
+      <c r="H43" t="s">
         <v>29</v>
       </c>
-      <c r="I40" t="s">
+      <c r="I43" t="s">
         <v>50</v>
       </c>
-      <c r="J40" t="s">
+      <c r="J43" t="s">
         <v>22</v>
       </c>
-      <c r="K40" t="s">
+      <c r="K43" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
+    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
         <v>24</v>
       </c>
-      <c r="C41">
-        <v>1</v>
-      </c>
-      <c r="D41">
+      <c r="C44">
+        <v>1</v>
+      </c>
+      <c r="D44">
         <f>IF(OR(AND(Tabelle5[[#This Row],[FTR/RET]]&lt;=1, Tabelle5[[#This Row],[DET]] &lt;= 15), AND(Tabelle5[[#This Row],[FTR/RET]]&lt;= 3, Tabelle5[[#This Row],[DET]] &lt;= 4)), 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="E41">
+      <c r="E44">
         <f>IF(OR(AND(Tabelle5[[#This Row],[FTR/RET]]&lt;=1, Tabelle5[[#This Row],[DET]] &gt; 15), AND(Tabelle5[[#This Row],[FTR/RET]]&lt;=5, Tabelle5[[#This Row],[FTR/RET]]&gt;=2, Tabelle5[[#This Row],[DET]] &gt;= 5, Tabelle5[[#This Row],[DET]] &lt;= 15), AND(Tabelle5[[#This Row],[FTR/RET]] &gt;= 5, Tabelle5[[#This Row],[DET]] &lt;= 4 )), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="F41">
+      <c r="F44">
         <f>IF(AND(Tabelle5[[#This Row],[Simple]]=0,Tabelle5[[#This Row],[Average]]=0), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="G41">
-        <v>1</v>
-      </c>
-      <c r="H41">
-        <v>1</v>
-      </c>
-      <c r="I41">
+      <c r="G44">
+        <v>1</v>
+      </c>
+      <c r="H44">
+        <v>1</v>
+      </c>
+      <c r="I44">
         <f>Tabelle5[[#This Row],[Count]]*(3*Tabelle5[[#This Row],[Simple]]+4*Tabelle5[[#This Row],[Average]]+6*Tabelle5[[#This Row],[Complex]])</f>
         <v>3</v>
       </c>
-      <c r="J41" t="s">
+      <c r="J44" t="s">
         <v>38</v>
       </c>
-      <c r="K41">
+      <c r="K44">
         <f>SUM(Tabelle5[Points])*(0.65+(5)/100)</f>
         <v>18.900000000000002</v>
       </c>
     </row>
-    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
+    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
         <v>25</v>
       </c>
-      <c r="C42">
-        <v>0</v>
-      </c>
-      <c r="D42">
+      <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="D45">
         <f>IF(OR(AND(Tabelle5[[#This Row],[FTR/RET]]&lt;=1, Tabelle5[[#This Row],[DET]] &lt;= 19), AND(Tabelle5[[#This Row],[FTR/RET]]&lt;= 3, Tabelle5[[#This Row],[DET]] &lt;= 5)), 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="E42">
+      <c r="E45">
         <f>IF(OR(AND(Tabelle5[[#This Row],[FTR/RET]]&lt;=1, Tabelle5[[#This Row],[DET]] &gt; 20), AND(Tabelle5[[#This Row],[FTR/RET]]&lt;=5, Tabelle5[[#This Row],[FTR/RET]]&gt;=2, Tabelle5[[#This Row],[DET]] &gt;= 6, Tabelle5[[#This Row],[DET]] &lt;= 19), AND(Tabelle5[[#This Row],[FTR/RET]] &gt;= 5, Tabelle5[[#This Row],[DET]] &lt;= 5 )), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="F42">
+      <c r="F45">
         <f>IF(AND(Tabelle5[[#This Row],[Simple]]=0,Tabelle5[[#This Row],[Average]]=0), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="G42">
-        <v>0</v>
-      </c>
-      <c r="H42">
-        <v>0</v>
-      </c>
-      <c r="I42">
+      <c r="G45">
+        <v>0</v>
+      </c>
+      <c r="H45">
+        <v>0</v>
+      </c>
+      <c r="I45">
         <f>Tabelle5[[#This Row],[Count]]*(Tabelle5[[#This Row],[Simple]]*4+Tabelle5[[#This Row],[Average]]*5+Tabelle5[[#This Row],[Complex]]*7)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
+    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
         <v>26</v>
       </c>
-      <c r="C43">
-        <v>1</v>
-      </c>
-      <c r="D43">
+      <c r="C46">
+        <v>1</v>
+      </c>
+      <c r="D46">
         <f>IF(OR(AND(Tabelle5[[#This Row],[FTR/RET]]&lt;=1, Tabelle5[[#This Row],[DET]] &lt;= 19), AND(Tabelle5[[#This Row],[FTR/RET]]&lt;= 3, Tabelle5[[#This Row],[DET]] &lt;= 5)), 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="E43">
+      <c r="E46">
         <f>IF(OR(AND(Tabelle5[[#This Row],[FTR/RET]]&lt;=1, Tabelle5[[#This Row],[DET]] &gt; 20), AND(Tabelle5[[#This Row],[FTR/RET]]&lt;=5, Tabelle5[[#This Row],[FTR/RET]]&gt;=2, Tabelle5[[#This Row],[DET]] &gt;= 6, Tabelle5[[#This Row],[DET]] &lt;= 19), AND(Tabelle5[[#This Row],[FTR/RET]] &gt;= 5, Tabelle5[[#This Row],[DET]] &lt;= 5 )), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="F43">
+      <c r="F46">
         <f>IF(AND(Tabelle5[[#This Row],[Simple]]=0,Tabelle5[[#This Row],[Average]]=0), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="G43">
-        <v>0</v>
-      </c>
-      <c r="H43">
-        <v>0</v>
-      </c>
-      <c r="I43">
+      <c r="G46">
+        <v>0</v>
+      </c>
+      <c r="H46">
+        <v>0</v>
+      </c>
+      <c r="I46">
         <f>Tabelle5[[#This Row],[Count]]*(3*Tabelle5[[#This Row],[Simple]]+4*Tabelle5[[#This Row],[Average]]+6*Tabelle5[[#This Row],[Complex]])</f>
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
+    <row r="47" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
         <v>27</v>
       </c>
-      <c r="C44">
+      <c r="C47">
         <v>3</v>
       </c>
-      <c r="D44">
+      <c r="D47">
         <f>IF(OR(AND(Tabelle5[[#This Row],[FTR/RET]]&lt;2, Tabelle5[[#This Row],[DET]] &lt;= 50), AND(Tabelle5[[#This Row],[FTR/RET]]&lt;=5, Tabelle5[[#This Row],[DET]] &lt; 20)), 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="E44">
+      <c r="E47">
         <f>IF(OR(AND(Tabelle5[[#This Row],[FTR/RET]]=1, Tabelle5[[#This Row],[DET]] &gt; 50), AND(Tabelle5[[#This Row],[FTR/RET]]&lt;=5, Tabelle5[[#This Row],[FTR/RET]]&gt;=2, Tabelle5[[#This Row],[DET]] &gt;= 20, Tabelle5[[#This Row],[DET]] &lt;= 50), AND(Tabelle5[[#This Row],[FTR/RET]] &gt;= 5, Tabelle5[[#This Row],[DET]] &lt; 20)), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="F44">
+      <c r="F47">
         <f>IF(AND(Tabelle5[[#This Row],[Simple]]=0,Tabelle5[[#This Row],[Average]]=0), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="G44">
-        <v>0</v>
-      </c>
-      <c r="H44">
-        <v>0</v>
-      </c>
-      <c r="I44">
+      <c r="G47">
+        <v>0</v>
+      </c>
+      <c r="H47">
+        <v>0</v>
+      </c>
+      <c r="I47">
         <f>Tabelle5[[#This Row],[Count]]*(7*Tabelle5[[#This Row],[Simple]]+10*Tabelle5[[#This Row],[Average]]+15*Tabelle5[[#This Row],[Complex]])</f>
         <v>21</v>
       </c>
-      <c r="J44" t="s">
+      <c r="J47" t="s">
         <v>56</v>
-      </c>
-    </row>
-    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
-        <v>28</v>
-      </c>
-      <c r="C45">
-        <v>0</v>
-      </c>
-      <c r="D45">
-        <f>IF(OR(AND(Tabelle5[[#This Row],[FTR/RET]]&lt;2, Tabelle5[[#This Row],[DET]] &lt;= 50), AND(Tabelle5[[#This Row],[FTR/RET]]&lt;=5, Tabelle5[[#This Row],[DET]] &lt; 20)), 1, 0)</f>
-        <v>1</v>
-      </c>
-      <c r="E45">
-        <f>IF(OR(AND(Tabelle5[[#This Row],[FTR/RET]]=1, Tabelle5[[#This Row],[DET]] &gt; 50), AND(Tabelle5[[#This Row],[FTR/RET]]&lt;=5, Tabelle5[[#This Row],[FTR/RET]]&gt;=2, Tabelle5[[#This Row],[DET]] &gt;= 20, Tabelle5[[#This Row],[DET]] &lt;= 50), AND(Tabelle5[[#This Row],[FTR/RET]] &gt;= 5, Tabelle5[[#This Row],[DET]] &lt; 20)), 1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="F45">
-        <f>IF(AND(Tabelle5[[#This Row],[Simple]]=0,Tabelle5[[#This Row],[Average]]=0), 1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="G45">
-        <v>0</v>
-      </c>
-      <c r="H45">
-        <v>0</v>
-      </c>
-      <c r="I45">
-        <f>Tabelle5[[#This Row],[Count]]*(5*Tabelle5[[#This Row],[Simple]]+7*Tabelle5[[#This Row],[Average]]+10*Tabelle5[[#This Row],[Complex]])</f>
-        <v>0</v>
       </c>
     </row>
     <row r="48" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
+        <v>28</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
+      </c>
+      <c r="D48">
+        <f>IF(OR(AND(Tabelle5[[#This Row],[FTR/RET]]&lt;2, Tabelle5[[#This Row],[DET]] &lt;= 50), AND(Tabelle5[[#This Row],[FTR/RET]]&lt;=5, Tabelle5[[#This Row],[DET]] &lt; 20)), 1, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="E48">
+        <f>IF(OR(AND(Tabelle5[[#This Row],[FTR/RET]]=1, Tabelle5[[#This Row],[DET]] &gt; 50), AND(Tabelle5[[#This Row],[FTR/RET]]&lt;=5, Tabelle5[[#This Row],[FTR/RET]]&gt;=2, Tabelle5[[#This Row],[DET]] &gt;= 20, Tabelle5[[#This Row],[DET]] &lt;= 50), AND(Tabelle5[[#This Row],[FTR/RET]] &gt;= 5, Tabelle5[[#This Row],[DET]] &lt; 20)), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="F48">
+        <f>IF(AND(Tabelle5[[#This Row],[Simple]]=0,Tabelle5[[#This Row],[Average]]=0), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="G48">
+        <v>0</v>
+      </c>
+      <c r="H48">
+        <v>0</v>
+      </c>
+      <c r="I48">
+        <f>Tabelle5[[#This Row],[Count]]*(5*Tabelle5[[#This Row],[Simple]]+7*Tabelle5[[#This Row],[Average]]+10*Tabelle5[[#This Row],[Complex]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
         <v>39</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C51" t="s">
         <v>21</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D51" t="s">
         <v>18</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E51" t="s">
         <v>19</v>
       </c>
-      <c r="F48" t="s">
+      <c r="F51" t="s">
         <v>20</v>
       </c>
-      <c r="G48" t="s">
+      <c r="G51" t="s">
         <v>49</v>
       </c>
-      <c r="H48" t="s">
+      <c r="H51" t="s">
         <v>29</v>
       </c>
-      <c r="I48" t="s">
+      <c r="I51" t="s">
         <v>50</v>
       </c>
-      <c r="J48" t="s">
+      <c r="J51" t="s">
         <v>22</v>
       </c>
-      <c r="K48" t="s">
+      <c r="K51" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="49" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B49" t="s">
+    <row r="52" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
         <v>24</v>
       </c>
-      <c r="C49">
-        <v>0</v>
-      </c>
-      <c r="D49">
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52">
         <f>IF(OR(AND(Tabelle6[[#This Row],[FTR/RET]]&lt;=1, Tabelle6[[#This Row],[DET]] &lt;= 15), AND(Tabelle6[[#This Row],[FTR/RET]]&lt;= 3, Tabelle6[[#This Row],[DET]] &lt;= 4)), 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="E49">
+      <c r="E52">
         <f>IF(OR(AND(Tabelle6[[#This Row],[FTR/RET]]&lt;=1, Tabelle6[[#This Row],[DET]] &gt; 15), AND(Tabelle6[[#This Row],[FTR/RET]]&lt;=5, Tabelle6[[#This Row],[FTR/RET]]&gt;=2, Tabelle6[[#This Row],[DET]] &gt;= 5, Tabelle6[[#This Row],[DET]] &lt;= 15), AND(Tabelle6[[#This Row],[FTR/RET]] &gt;= 5, Tabelle6[[#This Row],[DET]] &lt;= 4 )), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="F49">
+      <c r="F52">
         <f>IF(AND(Tabelle6[[#This Row],[Simple]]=0,Tabelle6[[#This Row],[Average]]=0), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="G49">
-        <v>0</v>
-      </c>
-      <c r="H49">
-        <v>0</v>
-      </c>
-      <c r="I49">
+      <c r="G52">
+        <v>0</v>
+      </c>
+      <c r="H52">
+        <v>0</v>
+      </c>
+      <c r="I52">
         <f>Tabelle6[[#This Row],[Count]]*(3*Tabelle6[[#This Row],[Simple]]+4*Tabelle6[[#This Row],[Average]]+6*Tabelle6[[#This Row],[Complex]])</f>
         <v>0</v>
       </c>
-      <c r="K49">
+      <c r="K52">
         <f>SUM(Tabelle6[Points])*0.65</f>
         <v>13.65</v>
       </c>
     </row>
-    <row r="50" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B50" t="s">
+    <row r="53" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
         <v>25</v>
       </c>
-      <c r="C50">
-        <v>1</v>
-      </c>
-      <c r="D50">
+      <c r="C53">
+        <v>1</v>
+      </c>
+      <c r="D53">
         <f>IF(OR(AND(Tabelle6[[#This Row],[FTR/RET]]&lt;=1, Tabelle6[[#This Row],[DET]] &lt;= 19), AND(Tabelle6[[#This Row],[FTR/RET]]&lt;= 3, Tabelle6[[#This Row],[DET]] &lt;= 5)), 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="E50">
+      <c r="E53">
         <f>IF(OR(AND(Tabelle6[[#This Row],[FTR/RET]]&lt;=1, Tabelle6[[#This Row],[DET]] &gt; 20), AND(Tabelle6[[#This Row],[FTR/RET]]&lt;=5, Tabelle6[[#This Row],[FTR/RET]]&gt;=2, Tabelle6[[#This Row],[DET]] &gt;= 6, Tabelle6[[#This Row],[DET]] &lt;= 19), AND(Tabelle6[[#This Row],[FTR/RET]] &gt;= 5, Tabelle6[[#This Row],[DET]] &lt;= 5 )), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="F50">
+      <c r="F53">
         <f>IF(AND(Tabelle6[[#This Row],[Simple]]=0,Tabelle6[[#This Row],[Average]]=0), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="G50">
-        <v>0</v>
-      </c>
-      <c r="H50">
+      <c r="G53">
+        <v>0</v>
+      </c>
+      <c r="H53">
         <v>2</v>
       </c>
-      <c r="I50">
+      <c r="I53">
         <f>Tabelle6[[#This Row],[Count]]*(Tabelle6[[#This Row],[Simple]]*4+Tabelle6[[#This Row],[Average]]*5+Tabelle6[[#This Row],[Complex]]*7)</f>
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
+    <row r="54" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
         <v>26</v>
       </c>
-      <c r="C51">
-        <v>1</v>
-      </c>
-      <c r="D51">
+      <c r="C54">
+        <v>1</v>
+      </c>
+      <c r="D54">
         <f>IF(OR(AND(Tabelle6[[#This Row],[FTR/RET]]&lt;=1, Tabelle6[[#This Row],[DET]] &lt;= 19), AND(Tabelle6[[#This Row],[FTR/RET]]&lt;= 3, Tabelle6[[#This Row],[DET]] &lt;= 5)), 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="E51">
+      <c r="E54">
         <f>IF(OR(AND(Tabelle6[[#This Row],[FTR/RET]]&lt;=1, Tabelle6[[#This Row],[DET]] &gt; 20), AND(Tabelle6[[#This Row],[FTR/RET]]&lt;=5, Tabelle6[[#This Row],[FTR/RET]]&gt;=2, Tabelle6[[#This Row],[DET]] &gt;= 6, Tabelle6[[#This Row],[DET]] &lt;= 19), AND(Tabelle6[[#This Row],[FTR/RET]] &gt;= 5, Tabelle6[[#This Row],[DET]] &lt;= 5 )), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="F51">
+      <c r="F54">
         <f>IF(AND(Tabelle6[[#This Row],[Simple]]=0,Tabelle6[[#This Row],[Average]]=0), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="G51">
-        <v>0</v>
-      </c>
-      <c r="H51">
-        <v>1</v>
-      </c>
-      <c r="I51">
+      <c r="G54">
+        <v>0</v>
+      </c>
+      <c r="H54">
+        <v>1</v>
+      </c>
+      <c r="I54">
         <f>Tabelle6[[#This Row],[Count]]*(3*Tabelle6[[#This Row],[Simple]]+4*Tabelle6[[#This Row],[Average]]+6*Tabelle6[[#This Row],[Complex]])</f>
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B52" t="s">
+    <row r="55" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
         <v>27</v>
       </c>
-      <c r="C52">
+      <c r="C55">
         <v>2</v>
       </c>
-      <c r="D52">
+      <c r="D55">
         <f>IF(OR(AND(Tabelle6[[#This Row],[FTR/RET]]&lt;2, Tabelle6[[#This Row],[DET]] &lt;= 50), AND(Tabelle6[[#This Row],[FTR/RET]]&lt;=5, Tabelle6[[#This Row],[DET]] &lt; 20)), 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="E52">
+      <c r="E55">
         <f>IF(OR(AND(Tabelle6[[#This Row],[FTR/RET]]=1, Tabelle6[[#This Row],[DET]] &gt; 50), AND(Tabelle6[[#This Row],[FTR/RET]]&lt;=5, Tabelle6[[#This Row],[FTR/RET]]&gt;=2, Tabelle6[[#This Row],[DET]] &gt;= 20, Tabelle6[[#This Row],[DET]] &lt;= 50), AND(Tabelle6[[#This Row],[FTR/RET]] &gt;= 5, Tabelle6[[#This Row],[DET]] &lt; 20)), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="F52">
+      <c r="F55">
         <f>IF(AND(Tabelle6[[#This Row],[Simple]]=0,Tabelle6[[#This Row],[Average]]=0), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="G52">
-        <v>0</v>
-      </c>
-      <c r="H52">
+      <c r="G55">
+        <v>0</v>
+      </c>
+      <c r="H55">
         <v>2</v>
       </c>
-      <c r="I52">
+      <c r="I55">
         <f>Tabelle6[[#This Row],[Count]]*(7*Tabelle6[[#This Row],[Simple]]+10*Tabelle6[[#This Row],[Average]]+15*Tabelle6[[#This Row],[Complex]])</f>
         <v>14</v>
       </c>
-      <c r="J52" t="s">
+      <c r="J55" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="53" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
-        <v>28</v>
-      </c>
-      <c r="C53">
-        <v>0</v>
-      </c>
-      <c r="D53">
-        <f>IF(OR(AND(Tabelle6[[#This Row],[FTR/RET]]&lt;2, Tabelle6[[#This Row],[DET]] &lt;= 50), AND(Tabelle6[[#This Row],[FTR/RET]]&lt;=5, Tabelle6[[#This Row],[DET]] &lt; 20)), 1, 0)</f>
-        <v>1</v>
-      </c>
-      <c r="E53">
-        <f>IF(OR(AND(Tabelle6[[#This Row],[FTR/RET]]=1, Tabelle6[[#This Row],[DET]] &gt; 50), AND(Tabelle6[[#This Row],[FTR/RET]]&lt;=5, Tabelle6[[#This Row],[FTR/RET]]&gt;=2, Tabelle6[[#This Row],[DET]] &gt;= 20, Tabelle6[[#This Row],[DET]] &lt;= 50), AND(Tabelle6[[#This Row],[FTR/RET]] &gt;= 5, Tabelle6[[#This Row],[DET]] &lt; 20)), 1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="F53">
-        <f>IF(AND(Tabelle6[[#This Row],[Simple]]=0,Tabelle6[[#This Row],[Average]]=0), 1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="G53">
-        <v>0</v>
-      </c>
-      <c r="H53">
-        <v>0</v>
-      </c>
-      <c r="I53">
-        <f>Tabelle6[[#This Row],[Count]]*(5*Tabelle6[[#This Row],[Simple]]+7*Tabelle6[[#This Row],[Average]]+10*Tabelle6[[#This Row],[Complex]])</f>
-        <v>0</v>
       </c>
     </row>
     <row r="56" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
+        <v>28</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <f>IF(OR(AND(Tabelle6[[#This Row],[FTR/RET]]&lt;2, Tabelle6[[#This Row],[DET]] &lt;= 50), AND(Tabelle6[[#This Row],[FTR/RET]]&lt;=5, Tabelle6[[#This Row],[DET]] &lt; 20)), 1, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="E56">
+        <f>IF(OR(AND(Tabelle6[[#This Row],[FTR/RET]]=1, Tabelle6[[#This Row],[DET]] &gt; 50), AND(Tabelle6[[#This Row],[FTR/RET]]&lt;=5, Tabelle6[[#This Row],[FTR/RET]]&gt;=2, Tabelle6[[#This Row],[DET]] &gt;= 20, Tabelle6[[#This Row],[DET]] &lt;= 50), AND(Tabelle6[[#This Row],[FTR/RET]] &gt;= 5, Tabelle6[[#This Row],[DET]] &lt; 20)), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="F56">
+        <f>IF(AND(Tabelle6[[#This Row],[Simple]]=0,Tabelle6[[#This Row],[Average]]=0), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="G56">
+        <v>0</v>
+      </c>
+      <c r="H56">
+        <v>0</v>
+      </c>
+      <c r="I56">
+        <f>Tabelle6[[#This Row],[Count]]*(5*Tabelle6[[#This Row],[Simple]]+7*Tabelle6[[#This Row],[Average]]+10*Tabelle6[[#This Row],[Complex]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
         <v>11</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C59" t="s">
         <v>21</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D59" t="s">
         <v>18</v>
       </c>
-      <c r="E56" t="s">
+      <c r="E59" t="s">
         <v>19</v>
       </c>
-      <c r="F56" t="s">
+      <c r="F59" t="s">
         <v>20</v>
       </c>
-      <c r="G56" t="s">
+      <c r="G59" t="s">
         <v>49</v>
       </c>
-      <c r="H56" t="s">
+      <c r="H59" t="s">
         <v>29</v>
       </c>
-      <c r="I56" t="s">
+      <c r="I59" t="s">
         <v>50</v>
       </c>
-      <c r="J56" t="s">
+      <c r="J59" t="s">
         <v>22</v>
       </c>
-      <c r="K56" t="s">
+      <c r="K59" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="57" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B57" t="s">
+    <row r="60" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
         <v>24</v>
       </c>
-      <c r="C57">
-        <v>0</v>
-      </c>
-      <c r="D57">
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60">
         <f>IF(OR(AND(Tabelle7[[#This Row],[FTR/RET]]&lt;=1, Tabelle7[[#This Row],[DET]] &lt;= 15), AND(Tabelle7[[#This Row],[FTR/RET]]&lt;= 3, Tabelle7[[#This Row],[DET]] &lt;= 4)), 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="E57">
+      <c r="E60">
         <f>IF(OR(AND(Tabelle7[[#This Row],[FTR/RET]]&lt;=1, Tabelle7[[#This Row],[DET]] &gt; 15), AND(Tabelle7[[#This Row],[FTR/RET]]&lt;=5, Tabelle7[[#This Row],[FTR/RET]]&gt;=2, Tabelle7[[#This Row],[DET]] &gt;= 5, Tabelle7[[#This Row],[DET]] &lt;= 15), AND(Tabelle7[[#This Row],[FTR/RET]] &gt;= 5, Tabelle7[[#This Row],[DET]] &lt;= 4 )), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="F57">
+      <c r="F60">
         <f>IF(AND(Tabelle7[[#This Row],[Simple]]=0,Tabelle7[[#This Row],[Average]]=0), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="G57">
-        <v>0</v>
-      </c>
-      <c r="H57">
-        <v>0</v>
-      </c>
-      <c r="I57">
+      <c r="G60">
+        <v>0</v>
+      </c>
+      <c r="H60">
+        <v>0</v>
+      </c>
+      <c r="I60">
         <f>Tabelle7[[#This Row],[Count]]*(3*Tabelle7[[#This Row],[Simple]]+4*Tabelle7[[#This Row],[Average]]+6*Tabelle7[[#This Row],[Complex]])</f>
         <v>0</v>
       </c>
-      <c r="K57">
+      <c r="K60">
         <f>SUM(Tabelle7[Points])*0.65</f>
         <v>18.2</v>
       </c>
     </row>
-    <row r="58" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B58" t="s">
+    <row r="61" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
         <v>25</v>
       </c>
-      <c r="C58">
-        <v>1</v>
-      </c>
-      <c r="D58">
+      <c r="C61">
+        <v>1</v>
+      </c>
+      <c r="D61">
         <f>IF(OR(AND(Tabelle7[[#This Row],[FTR/RET]]&lt;=1, Tabelle7[[#This Row],[DET]] &lt;= 19), AND(Tabelle7[[#This Row],[FTR/RET]]&lt;= 3, Tabelle7[[#This Row],[DET]] &lt;= 5)), 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="E58">
+      <c r="E61">
         <f>IF(OR(AND(Tabelle7[[#This Row],[FTR/RET]]&lt;=1, Tabelle7[[#This Row],[DET]] &gt; 20), AND(Tabelle7[[#This Row],[FTR/RET]]&lt;=5, Tabelle7[[#This Row],[FTR/RET]]&gt;=2, Tabelle7[[#This Row],[DET]] &gt;= 6, Tabelle7[[#This Row],[DET]] &lt;= 19), AND(Tabelle7[[#This Row],[FTR/RET]] &gt;= 5, Tabelle7[[#This Row],[DET]] &lt;= 5 )), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="F58">
+      <c r="F61">
         <f>IF(AND(Tabelle7[[#This Row],[Simple]]=0,Tabelle7[[#This Row],[Average]]=0), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="G58">
-        <v>0</v>
-      </c>
-      <c r="H58">
+      <c r="G61">
+        <v>0</v>
+      </c>
+      <c r="H61">
         <v>5</v>
       </c>
-      <c r="I58">
+      <c r="I61">
         <f>Tabelle7[[#This Row],[Count]]*(Tabelle7[[#This Row],[Simple]]*4+Tabelle7[[#This Row],[Average]]*5+Tabelle7[[#This Row],[Complex]]*7)</f>
         <v>4</v>
       </c>
     </row>
-    <row r="59" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B59" t="s">
+    <row r="62" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
         <v>26</v>
       </c>
-      <c r="C59">
-        <v>1</v>
-      </c>
-      <c r="D59">
+      <c r="C62">
+        <v>1</v>
+      </c>
+      <c r="D62">
         <f>IF(OR(AND(Tabelle7[[#This Row],[FTR/RET]]&lt;=1, Tabelle7[[#This Row],[DET]] &lt;= 19), AND(Tabelle7[[#This Row],[FTR/RET]]&lt;= 3, Tabelle7[[#This Row],[DET]] &lt;= 5)), 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="E59">
+      <c r="E62">
         <f>IF(OR(AND(Tabelle7[[#This Row],[FTR/RET]]&lt;=1, Tabelle7[[#This Row],[DET]] &gt; 20), AND(Tabelle7[[#This Row],[FTR/RET]]&lt;=5, Tabelle7[[#This Row],[FTR/RET]]&gt;=2, Tabelle7[[#This Row],[DET]] &gt;= 6, Tabelle7[[#This Row],[DET]] &lt;= 19), AND(Tabelle7[[#This Row],[FTR/RET]] &gt;= 5, Tabelle7[[#This Row],[DET]] &lt;= 5 )), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="F59">
+      <c r="F62">
         <f>IF(AND(Tabelle7[[#This Row],[Simple]]=0,Tabelle7[[#This Row],[Average]]=0), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="G59">
+      <c r="G62">
         <v>2</v>
       </c>
-      <c r="H59">
-        <v>0</v>
-      </c>
-      <c r="I59">
+      <c r="H62">
+        <v>0</v>
+      </c>
+      <c r="I62">
         <f>Tabelle7[[#This Row],[Count]]*(3*Tabelle7[[#This Row],[Simple]]+4*Tabelle7[[#This Row],[Average]]+6*Tabelle7[[#This Row],[Complex]])</f>
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B60" t="s">
+    <row r="63" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
         <v>27</v>
       </c>
-      <c r="C60">
+      <c r="C63">
         <v>3</v>
       </c>
-      <c r="D60">
+      <c r="D63">
         <f>IF(OR(AND(Tabelle7[[#This Row],[FTR/RET]]&lt;2, Tabelle7[[#This Row],[DET]] &lt;= 50), AND(Tabelle7[[#This Row],[FTR/RET]]&lt;=5, Tabelle7[[#This Row],[DET]] &lt; 20)), 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="E60">
+      <c r="E63">
         <f>IF(OR(AND(Tabelle7[[#This Row],[FTR/RET]]=1, Tabelle7[[#This Row],[DET]] &gt; 50), AND(Tabelle7[[#This Row],[FTR/RET]]&lt;=5, Tabelle7[[#This Row],[FTR/RET]]&gt;=2, Tabelle7[[#This Row],[DET]] &gt;= 20, Tabelle7[[#This Row],[DET]] &lt;= 50), AND(Tabelle7[[#This Row],[FTR/RET]] &gt;= 5, Tabelle7[[#This Row],[DET]] &lt; 20)), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="F60">
+      <c r="F63">
         <f>IF(AND(Tabelle7[[#This Row],[Simple]]=0,Tabelle7[[#This Row],[Average]]=0), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="G60">
-        <v>0</v>
-      </c>
-      <c r="H60">
-        <v>0</v>
-      </c>
-      <c r="I60">
+      <c r="G63">
+        <v>0</v>
+      </c>
+      <c r="H63">
+        <v>0</v>
+      </c>
+      <c r="I63">
         <f>Tabelle7[[#This Row],[Count]]*(7*Tabelle7[[#This Row],[Simple]]+10*Tabelle7[[#This Row],[Average]]+15*Tabelle7[[#This Row],[Complex]])</f>
         <v>21</v>
       </c>
-      <c r="J60" t="s">
+      <c r="J63" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="61" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B61" t="s">
-        <v>28</v>
-      </c>
-      <c r="C61">
-        <v>0</v>
-      </c>
-      <c r="D61">
-        <f>IF(OR(AND(Tabelle7[[#This Row],[FTR/RET]]&lt;2, Tabelle7[[#This Row],[DET]] &lt;= 50), AND(Tabelle7[[#This Row],[FTR/RET]]&lt;=5, Tabelle7[[#This Row],[DET]] &lt; 20)), 1, 0)</f>
-        <v>1</v>
-      </c>
-      <c r="E61">
-        <f>IF(OR(AND(Tabelle7[[#This Row],[FTR/RET]]=1, Tabelle7[[#This Row],[DET]] &gt; 50), AND(Tabelle7[[#This Row],[FTR/RET]]&lt;=5, Tabelle7[[#This Row],[FTR/RET]]&gt;=2, Tabelle7[[#This Row],[DET]] &gt;= 20, Tabelle7[[#This Row],[DET]] &lt;= 50), AND(Tabelle7[[#This Row],[FTR/RET]] &gt;= 5, Tabelle7[[#This Row],[DET]] &lt; 20)), 1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="F61">
-        <f>IF(AND(Tabelle7[[#This Row],[Simple]]=0,Tabelle7[[#This Row],[Average]]=0), 1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="G61">
-        <v>0</v>
-      </c>
-      <c r="H61">
-        <v>0</v>
-      </c>
-      <c r="I61">
-        <f>Tabelle7[[#This Row],[Count]]*(5*Tabelle7[[#This Row],[Simple]]+7*Tabelle7[[#This Row],[Average]]+10*Tabelle7[[#This Row],[Complex]])</f>
-        <v>0</v>
       </c>
     </row>
     <row r="64" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
+        <v>28</v>
+      </c>
+      <c r="C64">
+        <v>0</v>
+      </c>
+      <c r="D64">
+        <f>IF(OR(AND(Tabelle7[[#This Row],[FTR/RET]]&lt;2, Tabelle7[[#This Row],[DET]] &lt;= 50), AND(Tabelle7[[#This Row],[FTR/RET]]&lt;=5, Tabelle7[[#This Row],[DET]] &lt; 20)), 1, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="E64">
+        <f>IF(OR(AND(Tabelle7[[#This Row],[FTR/RET]]=1, Tabelle7[[#This Row],[DET]] &gt; 50), AND(Tabelle7[[#This Row],[FTR/RET]]&lt;=5, Tabelle7[[#This Row],[FTR/RET]]&gt;=2, Tabelle7[[#This Row],[DET]] &gt;= 20, Tabelle7[[#This Row],[DET]] &lt;= 50), AND(Tabelle7[[#This Row],[FTR/RET]] &gt;= 5, Tabelle7[[#This Row],[DET]] &lt; 20)), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="F64">
+        <f>IF(AND(Tabelle7[[#This Row],[Simple]]=0,Tabelle7[[#This Row],[Average]]=0), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="G64">
+        <v>0</v>
+      </c>
+      <c r="H64">
+        <v>0</v>
+      </c>
+      <c r="I64">
+        <f>Tabelle7[[#This Row],[Count]]*(5*Tabelle7[[#This Row],[Simple]]+7*Tabelle7[[#This Row],[Average]]+10*Tabelle7[[#This Row],[Complex]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
         <v>41</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C67" t="s">
         <v>21</v>
       </c>
-      <c r="D64" t="s">
+      <c r="D67" t="s">
         <v>18</v>
       </c>
-      <c r="E64" t="s">
+      <c r="E67" t="s">
         <v>19</v>
       </c>
-      <c r="F64" t="s">
+      <c r="F67" t="s">
         <v>20</v>
       </c>
-      <c r="G64" t="s">
+      <c r="G67" t="s">
         <v>49</v>
       </c>
-      <c r="H64" t="s">
+      <c r="H67" t="s">
         <v>29</v>
       </c>
-      <c r="I64" t="s">
+      <c r="I67" t="s">
         <v>50</v>
       </c>
-      <c r="J64" t="s">
+      <c r="J67" t="s">
         <v>22</v>
       </c>
-      <c r="K64" t="s">
+      <c r="K67" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="65" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B65" t="s">
+    <row r="68" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
         <v>24</v>
       </c>
-      <c r="C65">
-        <v>1</v>
-      </c>
-      <c r="D65">
+      <c r="C68">
+        <v>1</v>
+      </c>
+      <c r="D68">
         <f>IF(OR(AND(Tabelle8[[#This Row],[FTR/RET]]&lt;=1, Tabelle8[[#This Row],[DET]] &lt;= 15), AND(Tabelle8[[#This Row],[FTR/RET]]&lt;= 3, Tabelle8[[#This Row],[DET]] &lt;= 4)), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="E65">
+      <c r="E68">
         <f>IF(OR(AND(Tabelle8[[#This Row],[FTR/RET]]&lt;=1, Tabelle8[[#This Row],[DET]] &gt; 15), AND(Tabelle8[[#This Row],[FTR/RET]]&lt;=5, Tabelle8[[#This Row],[FTR/RET]]&gt;=2, Tabelle8[[#This Row],[DET]] &gt;= 5, Tabelle8[[#This Row],[DET]] &lt;= 15), AND(Tabelle8[[#This Row],[FTR/RET]] &gt;= 5, Tabelle8[[#This Row],[DET]] &lt;= 4 )), 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="F65">
+      <c r="F68">
         <f>IF(AND(Tabelle8[[#This Row],[Simple]]=0,Tabelle8[[#This Row],[Average]]=0), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="G65">
-        <v>1</v>
-      </c>
-      <c r="H65">
+      <c r="G68">
+        <v>1</v>
+      </c>
+      <c r="H68">
         <v>25</v>
       </c>
-      <c r="I65">
+      <c r="I68">
         <f>Tabelle8[[#This Row],[Count]]*(3*Tabelle8[[#This Row],[Simple]]+4*Tabelle8[[#This Row],[Average]]+6*Tabelle8[[#This Row],[Complex]])</f>
         <v>4</v>
       </c>
-      <c r="J65" t="s">
+      <c r="J68" t="s">
         <v>52</v>
       </c>
-      <c r="K65">
+      <c r="K68">
         <f>SUM(Tabelle8[Points])*(0.65+(5)/100)</f>
         <v>17.5</v>
       </c>
     </row>
-    <row r="66" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B66" t="s">
+    <row r="69" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
         <v>25</v>
       </c>
-      <c r="C66">
-        <v>0</v>
-      </c>
-      <c r="D66">
+      <c r="C69">
+        <v>0</v>
+      </c>
+      <c r="D69">
         <f>IF(OR(AND(Tabelle8[[#This Row],[FTR/RET]]&lt;=1, Tabelle8[[#This Row],[DET]] &lt;= 19), AND(Tabelle8[[#This Row],[FTR/RET]]&lt;= 3, Tabelle8[[#This Row],[DET]] &lt;= 5)), 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="E66">
+      <c r="E69">
         <f>IF(OR(AND(Tabelle8[[#This Row],[FTR/RET]]&lt;=1, Tabelle8[[#This Row],[DET]] &gt; 20), AND(Tabelle8[[#This Row],[FTR/RET]]&lt;=5, Tabelle8[[#This Row],[FTR/RET]]&gt;=2, Tabelle8[[#This Row],[DET]] &gt;= 6, Tabelle8[[#This Row],[DET]] &lt;= 19), AND(Tabelle8[[#This Row],[FTR/RET]] &gt;= 5, Tabelle8[[#This Row],[DET]] &lt;= 5 )), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="F66">
+      <c r="F69">
         <f>IF(AND(Tabelle8[[#This Row],[Simple]]=0,Tabelle8[[#This Row],[Average]]=0), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="G66">
-        <v>0</v>
-      </c>
-      <c r="H66">
-        <v>0</v>
-      </c>
-      <c r="I66">
+      <c r="G69">
+        <v>0</v>
+      </c>
+      <c r="H69">
+        <v>0</v>
+      </c>
+      <c r="I69">
         <f>Tabelle8[[#This Row],[Count]]*(Tabelle8[[#This Row],[Simple]]*4+Tabelle8[[#This Row],[Average]]*5+Tabelle8[[#This Row],[Complex]]*7)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B67" t="s">
+    <row r="70" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
         <v>26</v>
       </c>
-      <c r="C67">
-        <v>0</v>
-      </c>
-      <c r="D67">
+      <c r="C70">
+        <v>0</v>
+      </c>
+      <c r="D70">
         <f>IF(OR(AND(Tabelle8[[#This Row],[FTR/RET]]&lt;=1, Tabelle8[[#This Row],[DET]] &lt;= 19), AND(Tabelle8[[#This Row],[FTR/RET]]&lt;= 3, Tabelle8[[#This Row],[DET]] &lt;= 5)), 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="E67">
+      <c r="E70">
         <f>IF(OR(AND(Tabelle8[[#This Row],[FTR/RET]]&lt;=1, Tabelle8[[#This Row],[DET]] &gt; 20), AND(Tabelle8[[#This Row],[FTR/RET]]&lt;=5, Tabelle8[[#This Row],[FTR/RET]]&gt;=2, Tabelle8[[#This Row],[DET]] &gt;= 6, Tabelle8[[#This Row],[DET]] &lt;= 19), AND(Tabelle8[[#This Row],[FTR/RET]] &gt;= 5, Tabelle8[[#This Row],[DET]] &lt;= 5 )), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="F67">
+      <c r="F70">
         <f>IF(AND(Tabelle8[[#This Row],[Simple]]=0,Tabelle8[[#This Row],[Average]]=0), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="G67">
-        <v>0</v>
-      </c>
-      <c r="H67">
-        <v>0</v>
-      </c>
-      <c r="I67">
+      <c r="G70">
+        <v>0</v>
+      </c>
+      <c r="H70">
+        <v>0</v>
+      </c>
+      <c r="I70">
         <f>Tabelle8[[#This Row],[Count]]*(3*Tabelle8[[#This Row],[Simple]]+4*Tabelle8[[#This Row],[Average]]+6*Tabelle8[[#This Row],[Complex]])</f>
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B68" t="s">
+    <row r="71" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
         <v>27</v>
       </c>
-      <c r="C68">
+      <c r="C71">
         <v>3</v>
       </c>
-      <c r="D68">
+      <c r="D71">
         <f>IF(OR(AND(Tabelle8[[#This Row],[FTR/RET]]&lt;2, Tabelle8[[#This Row],[DET]] &lt;= 50), AND(Tabelle8[[#This Row],[FTR/RET]]&lt;=5, Tabelle8[[#This Row],[DET]] &lt; 20)), 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="E68">
+      <c r="E71">
         <f>IF(OR(AND(Tabelle8[[#This Row],[FTR/RET]]=1, Tabelle8[[#This Row],[DET]] &gt; 50), AND(Tabelle8[[#This Row],[FTR/RET]]&lt;=5, Tabelle8[[#This Row],[FTR/RET]]&gt;=2, Tabelle8[[#This Row],[DET]] &gt;= 20, Tabelle8[[#This Row],[DET]] &lt;= 50), AND(Tabelle8[[#This Row],[FTR/RET]] &gt;= 5, Tabelle8[[#This Row],[DET]] &lt; 20)), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="F68">
+      <c r="F71">
         <f>IF(AND(Tabelle8[[#This Row],[Simple]]=0,Tabelle8[[#This Row],[Average]]=0), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="G68">
-        <v>1</v>
-      </c>
-      <c r="H68">
+      <c r="G71">
+        <v>1</v>
+      </c>
+      <c r="H71">
         <v>11</v>
       </c>
-      <c r="I68">
+      <c r="I71">
         <f>Tabelle8[[#This Row],[Count]]*(7*Tabelle8[[#This Row],[Simple]]+10*Tabelle8[[#This Row],[Average]]+15*Tabelle8[[#This Row],[Complex]])</f>
         <v>21</v>
       </c>
-      <c r="J68" t="s">
+      <c r="J71" t="s">
         <v>53</v>
-      </c>
-    </row>
-    <row r="69" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B69" t="s">
-        <v>28</v>
-      </c>
-      <c r="C69">
-        <v>0</v>
-      </c>
-      <c r="D69">
-        <f>IF(OR(AND(Tabelle8[[#This Row],[FTR/RET]]&lt;2, Tabelle8[[#This Row],[DET]] &lt;= 50), AND(Tabelle8[[#This Row],[FTR/RET]]&lt;=5, Tabelle8[[#This Row],[DET]] &lt; 20)), 1, 0)</f>
-        <v>1</v>
-      </c>
-      <c r="E69">
-        <f>IF(OR(AND(Tabelle8[[#This Row],[FTR/RET]]=1, Tabelle8[[#This Row],[DET]] &gt; 50), AND(Tabelle8[[#This Row],[FTR/RET]]&lt;=5, Tabelle8[[#This Row],[FTR/RET]]&gt;=2, Tabelle8[[#This Row],[DET]] &gt;= 20, Tabelle8[[#This Row],[DET]] &lt;= 50), AND(Tabelle8[[#This Row],[FTR/RET]] &gt;= 5, Tabelle8[[#This Row],[DET]] &lt; 20)), 1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="F69">
-        <f>IF(AND(Tabelle8[[#This Row],[Simple]]=0,Tabelle8[[#This Row],[Average]]=0), 1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="G69">
-        <v>0</v>
-      </c>
-      <c r="H69">
-        <v>0</v>
-      </c>
-      <c r="I69">
-        <f>Tabelle8[[#This Row],[Count]]*(5*Tabelle8[[#This Row],[Simple]]+7*Tabelle8[[#This Row],[Average]]+10*Tabelle8[[#This Row],[Complex]])</f>
-        <v>0</v>
       </c>
     </row>
     <row r="72" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
+        <v>28</v>
+      </c>
+      <c r="C72">
+        <v>0</v>
+      </c>
+      <c r="D72">
+        <f>IF(OR(AND(Tabelle8[[#This Row],[FTR/RET]]&lt;2, Tabelle8[[#This Row],[DET]] &lt;= 50), AND(Tabelle8[[#This Row],[FTR/RET]]&lt;=5, Tabelle8[[#This Row],[DET]] &lt; 20)), 1, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="E72">
+        <f>IF(OR(AND(Tabelle8[[#This Row],[FTR/RET]]=1, Tabelle8[[#This Row],[DET]] &gt; 50), AND(Tabelle8[[#This Row],[FTR/RET]]&lt;=5, Tabelle8[[#This Row],[FTR/RET]]&gt;=2, Tabelle8[[#This Row],[DET]] &gt;= 20, Tabelle8[[#This Row],[DET]] &lt;= 50), AND(Tabelle8[[#This Row],[FTR/RET]] &gt;= 5, Tabelle8[[#This Row],[DET]] &lt; 20)), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="F72">
+        <f>IF(AND(Tabelle8[[#This Row],[Simple]]=0,Tabelle8[[#This Row],[Average]]=0), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="G72">
+        <v>0</v>
+      </c>
+      <c r="H72">
+        <v>0</v>
+      </c>
+      <c r="I72">
+        <f>Tabelle8[[#This Row],[Count]]*(5*Tabelle8[[#This Row],[Simple]]+7*Tabelle8[[#This Row],[Average]]+10*Tabelle8[[#This Row],[Complex]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B75" t="s">
         <v>13</v>
       </c>
-      <c r="C72" t="s">
+      <c r="C75" t="s">
         <v>21</v>
       </c>
-      <c r="D72" t="s">
+      <c r="D75" t="s">
         <v>18</v>
       </c>
-      <c r="E72" t="s">
+      <c r="E75" t="s">
         <v>19</v>
       </c>
-      <c r="F72" t="s">
+      <c r="F75" t="s">
         <v>20</v>
       </c>
-      <c r="G72" t="s">
+      <c r="G75" t="s">
         <v>49</v>
       </c>
-      <c r="H72" t="s">
+      <c r="H75" t="s">
         <v>29</v>
       </c>
-      <c r="I72" t="s">
+      <c r="I75" t="s">
         <v>50</v>
       </c>
-      <c r="J72" t="s">
+      <c r="J75" t="s">
         <v>22</v>
       </c>
-      <c r="K72" t="s">
+      <c r="K75" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="73" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B73" t="s">
+    <row r="76" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B76" t="s">
         <v>24</v>
       </c>
-      <c r="C73">
-        <v>1</v>
-      </c>
-      <c r="D73">
+      <c r="C76">
+        <v>1</v>
+      </c>
+      <c r="D76">
         <f>IF(OR(AND(Tabelle9[[#This Row],[FTR/RET]]&lt;=1, Tabelle9[[#This Row],[DET]] &lt;= 15), AND(Tabelle9[[#This Row],[FTR/RET]]&lt;= 3, Tabelle9[[#This Row],[DET]] &lt;= 4)), 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="E73">
+      <c r="E76">
         <f>IF(OR(AND(Tabelle9[[#This Row],[FTR/RET]]&lt;=1, Tabelle9[[#This Row],[DET]] &gt; 15), AND(Tabelle9[[#This Row],[FTR/RET]]&lt;=5, Tabelle9[[#This Row],[FTR/RET]]&gt;=2, Tabelle9[[#This Row],[DET]] &gt;= 5, Tabelle9[[#This Row],[DET]] &lt;= 15), AND(Tabelle9[[#This Row],[FTR/RET]] &gt;= 5, Tabelle9[[#This Row],[DET]] &lt;= 4 )), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="F73">
+      <c r="F76">
         <f>IF(AND(Tabelle9[[#This Row],[Simple]]=0,Tabelle9[[#This Row],[Average]]=0), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="G73">
-        <v>0</v>
-      </c>
-      <c r="H73">
-        <v>1</v>
-      </c>
-      <c r="I73">
+      <c r="G76">
+        <v>0</v>
+      </c>
+      <c r="H76">
+        <v>1</v>
+      </c>
+      <c r="I76">
         <f>Tabelle9[[#This Row],[Count]]*(3*Tabelle9[[#This Row],[Simple]]+4*Tabelle9[[#This Row],[Average]]+6*Tabelle9[[#This Row],[Complex]])</f>
         <v>3</v>
       </c>
-      <c r="K73">
+      <c r="K76">
         <f>SUM(Tabelle9[Points])*0.65</f>
         <v>11.05</v>
       </c>
     </row>
-    <row r="74" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B74" t="s">
+    <row r="77" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
         <v>25</v>
       </c>
-      <c r="C74">
-        <v>0</v>
-      </c>
-      <c r="D74">
+      <c r="C77">
+        <v>0</v>
+      </c>
+      <c r="D77">
         <f>IF(OR(AND(Tabelle9[[#This Row],[FTR/RET]]&lt;=1, Tabelle9[[#This Row],[DET]] &lt;= 19), AND(Tabelle9[[#This Row],[FTR/RET]]&lt;= 3, Tabelle9[[#This Row],[DET]] &lt;= 5)), 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="E74">
+      <c r="E77">
         <f>IF(OR(AND(Tabelle9[[#This Row],[FTR/RET]]&lt;=1, Tabelle9[[#This Row],[DET]] &gt; 20), AND(Tabelle9[[#This Row],[FTR/RET]]&lt;=5, Tabelle9[[#This Row],[FTR/RET]]&gt;=2, Tabelle9[[#This Row],[DET]] &gt;= 6, Tabelle9[[#This Row],[DET]] &lt;= 19), AND(Tabelle9[[#This Row],[FTR/RET]] &gt;= 5, Tabelle9[[#This Row],[DET]] &lt;= 5 )), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="F74">
+      <c r="F77">
         <f>IF(AND(Tabelle9[[#This Row],[Simple]]=0,Tabelle9[[#This Row],[Average]]=0), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="G74">
-        <v>0</v>
-      </c>
-      <c r="H74">
-        <v>0</v>
-      </c>
-      <c r="I74">
+      <c r="G77">
+        <v>0</v>
+      </c>
+      <c r="H77">
+        <v>0</v>
+      </c>
+      <c r="I77">
         <f>Tabelle9[[#This Row],[Count]]*(Tabelle9[[#This Row],[Simple]]*4+Tabelle9[[#This Row],[Average]]*5+Tabelle9[[#This Row],[Complex]]*7)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B75" t="s">
+    <row r="78" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B78" t="s">
         <v>26</v>
       </c>
-      <c r="C75">
-        <v>0</v>
-      </c>
-      <c r="D75">
+      <c r="C78">
+        <v>0</v>
+      </c>
+      <c r="D78">
         <f>IF(OR(AND(Tabelle9[[#This Row],[FTR/RET]]&lt;=1, Tabelle9[[#This Row],[DET]] &lt;= 19), AND(Tabelle9[[#This Row],[FTR/RET]]&lt;= 3, Tabelle9[[#This Row],[DET]] &lt;= 5)), 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="E75">
+      <c r="E78">
         <f>IF(OR(AND(Tabelle9[[#This Row],[FTR/RET]]&lt;=1, Tabelle9[[#This Row],[DET]] &gt; 20), AND(Tabelle9[[#This Row],[FTR/RET]]&lt;=5, Tabelle9[[#This Row],[FTR/RET]]&gt;=2, Tabelle9[[#This Row],[DET]] &gt;= 6, Tabelle9[[#This Row],[DET]] &lt;= 19), AND(Tabelle9[[#This Row],[FTR/RET]] &gt;= 5, Tabelle9[[#This Row],[DET]] &lt;= 5 )), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="F75">
+      <c r="F78">
         <f>IF(AND(Tabelle9[[#This Row],[Simple]]=0,Tabelle9[[#This Row],[Average]]=0), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="G75">
-        <v>0</v>
-      </c>
-      <c r="H75">
-        <v>0</v>
-      </c>
-      <c r="I75">
+      <c r="G78">
+        <v>0</v>
+      </c>
+      <c r="H78">
+        <v>0</v>
+      </c>
+      <c r="I78">
         <f>Tabelle9[[#This Row],[Count]]*(3*Tabelle9[[#This Row],[Simple]]+4*Tabelle9[[#This Row],[Average]]+6*Tabelle9[[#This Row],[Complex]])</f>
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B76" t="s">
+    <row r="79" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B79" t="s">
         <v>27</v>
       </c>
-      <c r="C76">
+      <c r="C79">
         <v>2</v>
       </c>
-      <c r="D76">
+      <c r="D79">
         <f>IF(OR(AND(Tabelle9[[#This Row],[FTR/RET]]&lt;2, Tabelle9[[#This Row],[DET]] &lt;= 50), AND(Tabelle9[[#This Row],[FTR/RET]]&lt;=5, Tabelle9[[#This Row],[DET]] &lt; 20)), 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="E76">
+      <c r="E79">
         <f>IF(OR(AND(Tabelle9[[#This Row],[FTR/RET]]=1, Tabelle9[[#This Row],[DET]] &gt; 50), AND(Tabelle9[[#This Row],[FTR/RET]]&lt;=5, Tabelle9[[#This Row],[FTR/RET]]&gt;=2, Tabelle9[[#This Row],[DET]] &gt;= 20, Tabelle9[[#This Row],[DET]] &lt;= 50), AND(Tabelle9[[#This Row],[FTR/RET]] &gt;= 5, Tabelle9[[#This Row],[DET]] &lt; 20)), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="F76">
+      <c r="F79">
         <f>IF(AND(Tabelle9[[#This Row],[Simple]]=0,Tabelle9[[#This Row],[Average]]=0), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="G76">
-        <v>0</v>
-      </c>
-      <c r="H76">
-        <v>0</v>
-      </c>
-      <c r="I76">
+      <c r="G79">
+        <v>0</v>
+      </c>
+      <c r="H79">
+        <v>0</v>
+      </c>
+      <c r="I79">
         <f>Tabelle9[[#This Row],[Count]]*(7*Tabelle9[[#This Row],[Simple]]+10*Tabelle9[[#This Row],[Average]]+15*Tabelle9[[#This Row],[Complex]])</f>
         <v>14</v>
       </c>
-      <c r="J76" t="s">
+      <c r="J79" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="77" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B77" t="s">
-        <v>28</v>
-      </c>
-      <c r="C77">
-        <v>0</v>
-      </c>
-      <c r="D77">
-        <f>IF(OR(AND(Tabelle9[[#This Row],[FTR/RET]]&lt;2, Tabelle9[[#This Row],[DET]] &lt;= 50), AND(Tabelle9[[#This Row],[FTR/RET]]&lt;=5, Tabelle9[[#This Row],[DET]] &lt; 20)), 1, 0)</f>
-        <v>1</v>
-      </c>
-      <c r="E77">
-        <f>IF(OR(AND(Tabelle9[[#This Row],[FTR/RET]]=1, Tabelle9[[#This Row],[DET]] &gt; 50), AND(Tabelle9[[#This Row],[FTR/RET]]&lt;=5, Tabelle9[[#This Row],[FTR/RET]]&gt;=2, Tabelle9[[#This Row],[DET]] &gt;= 20, Tabelle9[[#This Row],[DET]] &lt;= 50), AND(Tabelle9[[#This Row],[FTR/RET]] &gt;= 5, Tabelle9[[#This Row],[DET]] &lt; 20)), 1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="F77">
-        <f>IF(AND(Tabelle9[[#This Row],[Simple]]=0,Tabelle9[[#This Row],[Average]]=0), 1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="G77">
-        <v>0</v>
-      </c>
-      <c r="H77">
-        <v>0</v>
-      </c>
-      <c r="I77">
-        <f>Tabelle9[[#This Row],[Count]]*(5*Tabelle9[[#This Row],[Simple]]+7*Tabelle9[[#This Row],[Average]]+10*Tabelle9[[#This Row],[Complex]])</f>
-        <v>0</v>
       </c>
     </row>
     <row r="80" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
+        <v>28</v>
+      </c>
+      <c r="C80">
+        <v>0</v>
+      </c>
+      <c r="D80">
+        <f>IF(OR(AND(Tabelle9[[#This Row],[FTR/RET]]&lt;2, Tabelle9[[#This Row],[DET]] &lt;= 50), AND(Tabelle9[[#This Row],[FTR/RET]]&lt;=5, Tabelle9[[#This Row],[DET]] &lt; 20)), 1, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="E80">
+        <f>IF(OR(AND(Tabelle9[[#This Row],[FTR/RET]]=1, Tabelle9[[#This Row],[DET]] &gt; 50), AND(Tabelle9[[#This Row],[FTR/RET]]&lt;=5, Tabelle9[[#This Row],[FTR/RET]]&gt;=2, Tabelle9[[#This Row],[DET]] &gt;= 20, Tabelle9[[#This Row],[DET]] &lt;= 50), AND(Tabelle9[[#This Row],[FTR/RET]] &gt;= 5, Tabelle9[[#This Row],[DET]] &lt; 20)), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="F80">
+        <f>IF(AND(Tabelle9[[#This Row],[Simple]]=0,Tabelle9[[#This Row],[Average]]=0), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="G80">
+        <v>0</v>
+      </c>
+      <c r="H80">
+        <v>0</v>
+      </c>
+      <c r="I80">
+        <f>Tabelle9[[#This Row],[Count]]*(5*Tabelle9[[#This Row],[Simple]]+7*Tabelle9[[#This Row],[Average]]+10*Tabelle9[[#This Row],[Complex]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B83" t="s">
         <v>14</v>
       </c>
-      <c r="C80" t="s">
+      <c r="C83" t="s">
         <v>21</v>
       </c>
-      <c r="D80" t="s">
+      <c r="D83" t="s">
         <v>18</v>
       </c>
-      <c r="E80" t="s">
+      <c r="E83" t="s">
         <v>19</v>
       </c>
-      <c r="F80" t="s">
+      <c r="F83" t="s">
         <v>20</v>
       </c>
-      <c r="G80" t="s">
+      <c r="G83" t="s">
         <v>49</v>
       </c>
-      <c r="H80" t="s">
+      <c r="H83" t="s">
         <v>29</v>
       </c>
-      <c r="I80" t="s">
+      <c r="I83" t="s">
         <v>50</v>
       </c>
-      <c r="J80" t="s">
+      <c r="J83" t="s">
         <v>22</v>
       </c>
-      <c r="K80" t="s">
+      <c r="K83" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="81" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B81" t="s">
+    <row r="84" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B84" t="s">
         <v>24</v>
       </c>
-      <c r="C81">
+      <c r="C84">
         <v>10</v>
       </c>
-      <c r="D81">
+      <c r="D84">
         <f>IF(OR(AND(Tabelle10[[#This Row],[FTR/RET]]&lt;=1, Tabelle10[[#This Row],[DET]] &lt;= 15), AND(Tabelle10[[#This Row],[FTR/RET]]&lt;= 3, Tabelle10[[#This Row],[DET]] &lt;= 4)), 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="E81">
+      <c r="E84">
         <f>IF(OR(AND(Tabelle10[[#This Row],[FTR/RET]]&lt;=1, Tabelle10[[#This Row],[DET]] &gt; 15), AND(Tabelle10[[#This Row],[FTR/RET]]&lt;=5, Tabelle10[[#This Row],[FTR/RET]]&gt;=2, Tabelle10[[#This Row],[DET]] &gt;= 5, Tabelle10[[#This Row],[DET]] &lt;= 15), AND(Tabelle10[[#This Row],[FTR/RET]] &gt;= 5, Tabelle10[[#This Row],[DET]] &lt;= 4 )), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="F81">
+      <c r="F84">
         <f>IF(AND(Tabelle10[[#This Row],[Simple]]=0,Tabelle10[[#This Row],[Average]]=0), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="G81">
-        <v>1</v>
-      </c>
-      <c r="H81">
+      <c r="G84">
+        <v>1</v>
+      </c>
+      <c r="H84">
         <v>10</v>
       </c>
-      <c r="I81">
+      <c r="I84">
         <f>Tabelle10[[#This Row],[Count]]*(3*Tabelle10[[#This Row],[Simple]]+4*Tabelle10[[#This Row],[Average]]+6*Tabelle10[[#This Row],[Complex]])</f>
         <v>30</v>
       </c>
-      <c r="K81">
+      <c r="K84">
         <f>SUM(Tabelle10[Points])*0.65</f>
         <v>28.6</v>
       </c>
     </row>
-    <row r="82" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B82" t="s">
+    <row r="85" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B85" t="s">
         <v>25</v>
       </c>
-      <c r="C82">
-        <v>0</v>
-      </c>
-      <c r="D82">
+      <c r="C85">
+        <v>0</v>
+      </c>
+      <c r="D85">
         <f>IF(OR(AND(Tabelle10[[#This Row],[FTR/RET]]&lt;=1, Tabelle10[[#This Row],[DET]] &lt;= 19), AND(Tabelle10[[#This Row],[FTR/RET]]&lt;= 3, Tabelle10[[#This Row],[DET]] &lt;= 5)), 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="E82">
+      <c r="E85">
         <f>IF(OR(AND(Tabelle10[[#This Row],[FTR/RET]]&lt;=1, Tabelle10[[#This Row],[DET]] &gt; 20), AND(Tabelle10[[#This Row],[FTR/RET]]&lt;=5, Tabelle10[[#This Row],[FTR/RET]]&gt;=2, Tabelle10[[#This Row],[DET]] &gt;= 6, Tabelle10[[#This Row],[DET]] &lt;= 19), AND(Tabelle10[[#This Row],[FTR/RET]] &gt;= 5, Tabelle10[[#This Row],[DET]] &lt;= 5 )), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="F82">
+      <c r="F85">
         <f>IF(AND(Tabelle10[[#This Row],[Simple]]=0,Tabelle10[[#This Row],[Average]]=0), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="G82">
-        <v>0</v>
-      </c>
-      <c r="H82">
-        <v>0</v>
-      </c>
-      <c r="I82">
+      <c r="G85">
+        <v>0</v>
+      </c>
+      <c r="H85">
+        <v>0</v>
+      </c>
+      <c r="I85">
         <f>Tabelle10[[#This Row],[Count]]*(Tabelle10[[#This Row],[Simple]]*4+Tabelle10[[#This Row],[Average]]*5+Tabelle10[[#This Row],[Complex]]*7)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B83" t="s">
+    <row r="86" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B86" t="s">
         <v>26</v>
       </c>
-      <c r="C83">
-        <v>0</v>
-      </c>
-      <c r="D83">
+      <c r="C86">
+        <v>0</v>
+      </c>
+      <c r="D86">
         <f>IF(OR(AND(Tabelle10[[#This Row],[FTR/RET]]&lt;=1, Tabelle10[[#This Row],[DET]] &lt;= 19), AND(Tabelle10[[#This Row],[FTR/RET]]&lt;= 3, Tabelle10[[#This Row],[DET]] &lt;= 5)), 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="E83">
+      <c r="E86">
         <f>IF(OR(AND(Tabelle10[[#This Row],[FTR/RET]]&lt;=1, Tabelle10[[#This Row],[DET]] &gt; 20), AND(Tabelle10[[#This Row],[FTR/RET]]&lt;=5, Tabelle10[[#This Row],[FTR/RET]]&gt;=2, Tabelle10[[#This Row],[DET]] &gt;= 6, Tabelle10[[#This Row],[DET]] &lt;= 19), AND(Tabelle10[[#This Row],[FTR/RET]] &gt;= 5, Tabelle10[[#This Row],[DET]] &lt;= 5 )), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="F83">
+      <c r="F86">
         <f>IF(AND(Tabelle10[[#This Row],[Simple]]=0,Tabelle10[[#This Row],[Average]]=0), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="G83">
-        <v>0</v>
-      </c>
-      <c r="H83">
-        <v>0</v>
-      </c>
-      <c r="I83">
+      <c r="G86">
+        <v>0</v>
+      </c>
+      <c r="H86">
+        <v>0</v>
+      </c>
+      <c r="I86">
         <f>Tabelle10[[#This Row],[Count]]*(3*Tabelle10[[#This Row],[Simple]]+4*Tabelle10[[#This Row],[Average]]+6*Tabelle10[[#This Row],[Complex]])</f>
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B84" t="s">
+    <row r="87" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B87" t="s">
         <v>27</v>
       </c>
-      <c r="C84">
+      <c r="C87">
         <v>2</v>
       </c>
-      <c r="D84">
+      <c r="D87">
         <f>IF(OR(AND(Tabelle10[[#This Row],[FTR/RET]]&lt;2, Tabelle10[[#This Row],[DET]] &lt;= 50), AND(Tabelle10[[#This Row],[FTR/RET]]&lt;=5, Tabelle10[[#This Row],[DET]] &lt; 20)), 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="E84">
+      <c r="E87">
         <f>IF(OR(AND(Tabelle10[[#This Row],[FTR/RET]]=1, Tabelle10[[#This Row],[DET]] &gt; 50), AND(Tabelle10[[#This Row],[FTR/RET]]&lt;=5, Tabelle10[[#This Row],[FTR/RET]]&gt;=2, Tabelle10[[#This Row],[DET]] &gt;= 20, Tabelle10[[#This Row],[DET]] &lt;= 50), AND(Tabelle10[[#This Row],[FTR/RET]] &gt;= 5, Tabelle10[[#This Row],[DET]] &lt; 20)), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="F84">
+      <c r="F87">
         <f>IF(AND(Tabelle10[[#This Row],[Simple]]=0,Tabelle10[[#This Row],[Average]]=0), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="G84">
-        <v>0</v>
-      </c>
-      <c r="H84">
-        <v>0</v>
-      </c>
-      <c r="I84">
+      <c r="G87">
+        <v>0</v>
+      </c>
+      <c r="H87">
+        <v>0</v>
+      </c>
+      <c r="I87">
         <f>Tabelle10[[#This Row],[Count]]*(7*Tabelle10[[#This Row],[Simple]]+10*Tabelle10[[#This Row],[Average]]+15*Tabelle10[[#This Row],[Complex]])</f>
         <v>14</v>
       </c>
-      <c r="J84" t="s">
+      <c r="J87" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="85" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B85" t="s">
-        <v>28</v>
-      </c>
-      <c r="C85">
-        <v>0</v>
-      </c>
-      <c r="D85">
-        <f>IF(OR(AND(Tabelle10[[#This Row],[FTR/RET]]&lt;2, Tabelle10[[#This Row],[DET]] &lt;= 50), AND(Tabelle10[[#This Row],[FTR/RET]]&lt;=5, Tabelle10[[#This Row],[DET]] &lt; 20)), 1, 0)</f>
-        <v>1</v>
-      </c>
-      <c r="E85">
-        <f>IF(OR(AND(Tabelle10[[#This Row],[FTR/RET]]=1, Tabelle10[[#This Row],[DET]] &gt; 50), AND(Tabelle10[[#This Row],[FTR/RET]]&lt;=5, Tabelle10[[#This Row],[FTR/RET]]&gt;=2, Tabelle10[[#This Row],[DET]] &gt;= 20, Tabelle10[[#This Row],[DET]] &lt;= 50), AND(Tabelle10[[#This Row],[FTR/RET]] &gt;= 5, Tabelle10[[#This Row],[DET]] &lt; 20)), 1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="F85">
-        <f>IF(AND(Tabelle10[[#This Row],[Simple]]=0,Tabelle10[[#This Row],[Average]]=0), 1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="G85">
-        <v>0</v>
-      </c>
-      <c r="H85">
-        <v>0</v>
-      </c>
-      <c r="I85">
-        <f>Tabelle10[[#This Row],[Count]]*(5*Tabelle10[[#This Row],[Simple]]+7*Tabelle10[[#This Row],[Average]]+10*Tabelle10[[#This Row],[Complex]])</f>
-        <v>0</v>
       </c>
     </row>
     <row r="88" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
+        <v>28</v>
+      </c>
+      <c r="C88">
+        <v>0</v>
+      </c>
+      <c r="D88">
+        <f>IF(OR(AND(Tabelle10[[#This Row],[FTR/RET]]&lt;2, Tabelle10[[#This Row],[DET]] &lt;= 50), AND(Tabelle10[[#This Row],[FTR/RET]]&lt;=5, Tabelle10[[#This Row],[DET]] &lt; 20)), 1, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="E88">
+        <f>IF(OR(AND(Tabelle10[[#This Row],[FTR/RET]]=1, Tabelle10[[#This Row],[DET]] &gt; 50), AND(Tabelle10[[#This Row],[FTR/RET]]&lt;=5, Tabelle10[[#This Row],[FTR/RET]]&gt;=2, Tabelle10[[#This Row],[DET]] &gt;= 20, Tabelle10[[#This Row],[DET]] &lt;= 50), AND(Tabelle10[[#This Row],[FTR/RET]] &gt;= 5, Tabelle10[[#This Row],[DET]] &lt; 20)), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="F88">
+        <f>IF(AND(Tabelle10[[#This Row],[Simple]]=0,Tabelle10[[#This Row],[Average]]=0), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="G88">
+        <v>0</v>
+      </c>
+      <c r="H88">
+        <v>0</v>
+      </c>
+      <c r="I88">
+        <f>Tabelle10[[#This Row],[Count]]*(5*Tabelle10[[#This Row],[Simple]]+7*Tabelle10[[#This Row],[Average]]+10*Tabelle10[[#This Row],[Complex]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B91" t="s">
         <v>43</v>
       </c>
-      <c r="C88" t="s">
+      <c r="C91" t="s">
         <v>21</v>
       </c>
-      <c r="D88" t="s">
+      <c r="D91" t="s">
         <v>18</v>
       </c>
-      <c r="E88" t="s">
+      <c r="E91" t="s">
         <v>19</v>
       </c>
-      <c r="F88" t="s">
+      <c r="F91" t="s">
         <v>20</v>
       </c>
-      <c r="G88" t="s">
+      <c r="G91" t="s">
         <v>49</v>
       </c>
-      <c r="H88" t="s">
+      <c r="H91" t="s">
         <v>29</v>
       </c>
-      <c r="I88" t="s">
+      <c r="I91" t="s">
         <v>50</v>
       </c>
-      <c r="J88" t="s">
+      <c r="J91" t="s">
         <v>22</v>
       </c>
-      <c r="K88" t="s">
+      <c r="K91" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="89" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B89" t="s">
+    <row r="92" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B92" t="s">
         <v>24</v>
       </c>
-      <c r="D89">
+      <c r="D92">
         <f>IF(OR(AND(Tabelle11[[#This Row],[FTR/RET]]&lt;=1, Tabelle11[[#This Row],[DET]] &lt;= 15), AND(Tabelle11[[#This Row],[FTR/RET]]&lt;= 3, Tabelle11[[#This Row],[DET]] &lt;= 4)), 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="E89">
+      <c r="E92">
         <f>IF(OR(AND(Tabelle11[[#This Row],[FTR/RET]]&lt;=1, Tabelle11[[#This Row],[DET]] &gt; 15), AND(Tabelle11[[#This Row],[FTR/RET]]&lt;=5, Tabelle11[[#This Row],[FTR/RET]]&gt;=2, Tabelle11[[#This Row],[DET]] &gt;= 5, Tabelle11[[#This Row],[DET]] &lt;= 15), AND(Tabelle11[[#This Row],[FTR/RET]] &gt;= 5, Tabelle11[[#This Row],[DET]] &lt;= 4 )), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="F89">
+      <c r="F92">
         <f>IF(AND(Tabelle11[[#This Row],[Simple]]=0,Tabelle11[[#This Row],[Average]]=0), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="G89">
-        <v>0</v>
-      </c>
-      <c r="H89">
-        <v>0</v>
-      </c>
-      <c r="I89">
+      <c r="G92">
+        <v>0</v>
+      </c>
+      <c r="H92">
+        <v>0</v>
+      </c>
+      <c r="I92">
         <f>Tabelle11[[#This Row],[Count]]*(3*Tabelle11[[#This Row],[Simple]]+4*Tabelle11[[#This Row],[Average]]+6*Tabelle11[[#This Row],[Complex]])</f>
         <v>0</v>
       </c>
-      <c r="K89">
+      <c r="K92">
         <f>SUM(Tabelle11[Points])*0.65</f>
         <v>20.150000000000002</v>
       </c>
     </row>
-    <row r="90" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B90" t="s">
+    <row r="93" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B93" t="s">
         <v>25</v>
       </c>
-      <c r="D90">
+      <c r="D93">
         <f>IF(OR(AND(Tabelle11[[#This Row],[FTR/RET]]&lt;=1, Tabelle11[[#This Row],[DET]] &lt;= 19), AND(Tabelle11[[#This Row],[FTR/RET]]&lt;= 3, Tabelle11[[#This Row],[DET]] &lt;= 5)), 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="E90">
+      <c r="E93">
         <f>IF(OR(AND(Tabelle11[[#This Row],[FTR/RET]]&lt;=1, Tabelle11[[#This Row],[DET]] &gt; 20), AND(Tabelle11[[#This Row],[FTR/RET]]&lt;=5, Tabelle11[[#This Row],[FTR/RET]]&gt;=2, Tabelle11[[#This Row],[DET]] &gt;= 6, Tabelle11[[#This Row],[DET]] &lt;= 19), AND(Tabelle11[[#This Row],[FTR/RET]] &gt;= 5, Tabelle11[[#This Row],[DET]] &lt;= 5 )), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="F90">
+      <c r="F93">
         <f>IF(AND(Tabelle11[[#This Row],[Simple]]=0,Tabelle11[[#This Row],[Average]]=0), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="G90">
-        <v>0</v>
-      </c>
-      <c r="H90">
-        <v>0</v>
-      </c>
-      <c r="I90">
+      <c r="G93">
+        <v>0</v>
+      </c>
+      <c r="H93">
+        <v>0</v>
+      </c>
+      <c r="I93">
         <f>Tabelle11[[#This Row],[Count]]*(Tabelle11[[#This Row],[Simple]]*4+Tabelle11[[#This Row],[Average]]*5+Tabelle11[[#This Row],[Complex]]*7)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B91" t="s">
+    <row r="94" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B94" t="s">
         <v>26</v>
       </c>
-      <c r="C91">
-        <v>1</v>
-      </c>
-      <c r="D91">
+      <c r="C94">
+        <v>1</v>
+      </c>
+      <c r="D94">
         <f>IF(OR(AND(Tabelle11[[#This Row],[FTR/RET]]&lt;=1, Tabelle11[[#This Row],[DET]] &lt;= 19), AND(Tabelle11[[#This Row],[FTR/RET]]&lt;= 3, Tabelle11[[#This Row],[DET]] &lt;= 5)), 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="E91">
+      <c r="E94">
         <f>IF(OR(AND(Tabelle11[[#This Row],[FTR/RET]]&lt;=1, Tabelle11[[#This Row],[DET]] &gt; 20), AND(Tabelle11[[#This Row],[FTR/RET]]&lt;=5, Tabelle11[[#This Row],[FTR/RET]]&gt;=2, Tabelle11[[#This Row],[DET]] &gt;= 6, Tabelle11[[#This Row],[DET]] &lt;= 19), AND(Tabelle11[[#This Row],[FTR/RET]] &gt;= 5, Tabelle11[[#This Row],[DET]] &lt;= 5 )), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="F91">
+      <c r="F94">
         <f>IF(AND(Tabelle11[[#This Row],[Simple]]=0,Tabelle11[[#This Row],[Average]]=0), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="G91">
-        <v>0</v>
-      </c>
-      <c r="H91">
-        <v>0</v>
-      </c>
-      <c r="I91">
+      <c r="G94">
+        <v>0</v>
+      </c>
+      <c r="H94">
+        <v>0</v>
+      </c>
+      <c r="I94">
         <f>Tabelle11[[#This Row],[Count]]*(3*Tabelle11[[#This Row],[Simple]]+4*Tabelle11[[#This Row],[Average]]+6*Tabelle11[[#This Row],[Complex]])</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="92" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B92" t="s">
+      <c r="K94">
+        <f>SeeMapsFP/Tabelle15[Velocity]</f>
+        <v>5.0812672176308542</v>
+      </c>
+    </row>
+    <row r="95" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B95" t="s">
         <v>27</v>
       </c>
-      <c r="C92">
+      <c r="C95">
         <v>3</v>
       </c>
-      <c r="D92">
+      <c r="D95">
         <f>IF(OR(AND(Tabelle11[[#This Row],[FTR/RET]]&lt;2, Tabelle11[[#This Row],[DET]] &lt;= 50), AND(Tabelle11[[#This Row],[FTR/RET]]&lt;=5, Tabelle11[[#This Row],[DET]] &lt; 20)), 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="E92">
+      <c r="E95">
         <f>IF(OR(AND(Tabelle11[[#This Row],[FTR/RET]]=1, Tabelle11[[#This Row],[DET]] &gt; 50), AND(Tabelle11[[#This Row],[FTR/RET]]&lt;=5, Tabelle11[[#This Row],[FTR/RET]]&gt;=2, Tabelle11[[#This Row],[DET]] &gt;= 20, Tabelle11[[#This Row],[DET]] &lt;= 50), AND(Tabelle11[[#This Row],[FTR/RET]] &gt;= 5, Tabelle11[[#This Row],[DET]] &lt; 20)), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="F92">
+      <c r="F95">
         <f>IF(AND(Tabelle11[[#This Row],[Simple]]=0,Tabelle11[[#This Row],[Average]]=0), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="G92">
-        <v>0</v>
-      </c>
-      <c r="H92">
-        <v>0</v>
-      </c>
-      <c r="I92">
+      <c r="G95">
+        <v>0</v>
+      </c>
+      <c r="H95">
+        <v>0</v>
+      </c>
+      <c r="I95">
         <f>Tabelle11[[#This Row],[Count]]*(7*Tabelle11[[#This Row],[Simple]]+10*Tabelle11[[#This Row],[Average]]+15*Tabelle11[[#This Row],[Complex]])</f>
         <v>21</v>
       </c>
-      <c r="J92" t="s">
+      <c r="J95" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="93" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B93" t="s">
+    <row r="96" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B96" t="s">
         <v>28</v>
       </c>
-      <c r="C93">
-        <v>1</v>
-      </c>
-      <c r="D93">
+      <c r="C96">
+        <v>1</v>
+      </c>
+      <c r="D96">
         <f>IF(OR(AND(Tabelle11[[#This Row],[FTR/RET]]&lt;2, Tabelle11[[#This Row],[DET]] &lt;= 50), AND(Tabelle11[[#This Row],[FTR/RET]]&lt;=5, Tabelle11[[#This Row],[DET]] &lt; 20)), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="E93">
+      <c r="E96">
         <f>IF(OR(AND(Tabelle11[[#This Row],[FTR/RET]]=1, Tabelle11[[#This Row],[DET]] &gt; 50), AND(Tabelle11[[#This Row],[FTR/RET]]&lt;=5, Tabelle11[[#This Row],[FTR/RET]]&gt;=2, Tabelle11[[#This Row],[DET]] &gt;= 20, Tabelle11[[#This Row],[DET]] &lt;= 50), AND(Tabelle11[[#This Row],[FTR/RET]] &gt;= 5, Tabelle11[[#This Row],[DET]] &lt; 20)), 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="F93">
+      <c r="F96">
         <f>IF(AND(Tabelle11[[#This Row],[Simple]]=0,Tabelle11[[#This Row],[Average]]=0), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="G93">
+      <c r="G96">
         <v>5</v>
       </c>
-      <c r="H93">
+      <c r="H96">
         <v>30</v>
       </c>
-      <c r="I93">
+      <c r="I96">
         <f>Tabelle11[[#This Row],[Count]]*(5*Tabelle11[[#This Row],[Simple]]+7*Tabelle11[[#This Row],[Average]]+10*Tabelle11[[#This Row],[Complex]])</f>
         <v>7</v>
       </c>
-      <c r="J93" t="s">
+      <c r="J96" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="96" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B96" t="s">
+    <row r="99" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B99" t="s">
         <v>45</v>
       </c>
-      <c r="C96" t="s">
+      <c r="C99" t="s">
         <v>21</v>
       </c>
-      <c r="D96" t="s">
+      <c r="D99" t="s">
         <v>18</v>
       </c>
-      <c r="E96" t="s">
+      <c r="E99" t="s">
         <v>19</v>
       </c>
-      <c r="F96" t="s">
+      <c r="F99" t="s">
         <v>20</v>
       </c>
-      <c r="G96" t="s">
+      <c r="G99" t="s">
         <v>49</v>
       </c>
-      <c r="H96" t="s">
+      <c r="H99" t="s">
         <v>29</v>
       </c>
-      <c r="I96" t="s">
+      <c r="I99" t="s">
         <v>50</v>
       </c>
-      <c r="J96" t="s">
+      <c r="J99" t="s">
         <v>22</v>
       </c>
-      <c r="K96" t="s">
+      <c r="K99" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="97" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B97" t="s">
+    <row r="100" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B100" t="s">
         <v>24</v>
       </c>
-      <c r="C97">
-        <v>1</v>
-      </c>
-      <c r="D97">
+      <c r="C100">
+        <v>1</v>
+      </c>
+      <c r="D100">
         <f>IF(OR(AND(Tabelle12[[#This Row],[FTR/RET]]&lt;=1, Tabelle12[[#This Row],[DET]] &lt;= 15), AND(Tabelle12[[#This Row],[FTR/RET]]&lt;= 3, Tabelle12[[#This Row],[DET]] &lt;= 4)), 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="E97">
+      <c r="E100">
         <f>IF(OR(AND(Tabelle12[[#This Row],[FTR/RET]]&lt;=1, Tabelle12[[#This Row],[DET]] &gt; 15), AND(Tabelle12[[#This Row],[FTR/RET]]&lt;=5, Tabelle12[[#This Row],[FTR/RET]]&gt;=2, Tabelle12[[#This Row],[DET]] &gt;= 5, Tabelle12[[#This Row],[DET]] &lt;= 15), AND(Tabelle12[[#This Row],[FTR/RET]] &gt;= 5, Tabelle12[[#This Row],[DET]] &lt;= 4 )), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="F97">
+      <c r="F100">
         <f>IF(AND(Tabelle12[[#This Row],[Simple]]=0,Tabelle12[[#This Row],[Average]]=0), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="G97">
-        <v>0</v>
-      </c>
-      <c r="H97">
-        <v>1</v>
-      </c>
-      <c r="I97">
+      <c r="G100">
+        <v>0</v>
+      </c>
+      <c r="H100">
+        <v>1</v>
+      </c>
+      <c r="I100">
         <f>Tabelle12[[#This Row],[Count]]*(3*Tabelle12[[#This Row],[Simple]]+4*Tabelle12[[#This Row],[Average]]+6*Tabelle12[[#This Row],[Complex]])</f>
         <v>3</v>
       </c>
-      <c r="J97" t="s">
+      <c r="J100" t="s">
         <v>46</v>
       </c>
-      <c r="K97">
+      <c r="K100">
         <f>SUM(Tabelle12[Points])*0.65</f>
         <v>11.05</v>
       </c>
     </row>
-    <row r="98" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B98" t="s">
+    <row r="101" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B101" t="s">
         <v>25</v>
       </c>
-      <c r="C98">
-        <v>0</v>
-      </c>
-      <c r="D98">
+      <c r="C101">
+        <v>0</v>
+      </c>
+      <c r="D101">
         <f>IF(OR(AND(Tabelle12[[#This Row],[FTR/RET]]&lt;=1, Tabelle12[[#This Row],[DET]] &lt;= 19), AND(Tabelle12[[#This Row],[FTR/RET]]&lt;= 3, Tabelle12[[#This Row],[DET]] &lt;= 5)), 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="E98">
+      <c r="E101">
         <f>IF(OR(AND(Tabelle12[[#This Row],[FTR/RET]]&lt;=1, Tabelle12[[#This Row],[DET]] &gt; 20), AND(Tabelle12[[#This Row],[FTR/RET]]&lt;=5, Tabelle12[[#This Row],[FTR/RET]]&gt;=2, Tabelle12[[#This Row],[DET]] &gt;= 6, Tabelle12[[#This Row],[DET]] &lt;= 19), AND(Tabelle12[[#This Row],[FTR/RET]] &gt;= 5, Tabelle12[[#This Row],[DET]] &lt;= 5 )), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="F98">
+      <c r="F101">
         <f>IF(AND(Tabelle12[[#This Row],[Simple]]=0,Tabelle12[[#This Row],[Average]]=0), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="G98">
-        <v>0</v>
-      </c>
-      <c r="H98">
-        <v>0</v>
-      </c>
-      <c r="I98">
+      <c r="G101">
+        <v>0</v>
+      </c>
+      <c r="H101">
+        <v>0</v>
+      </c>
+      <c r="I101">
         <f>Tabelle12[[#This Row],[Count]]*(Tabelle12[[#This Row],[Simple]]*4+Tabelle12[[#This Row],[Average]]*5+Tabelle12[[#This Row],[Complex]]*7)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B99" t="s">
+    <row r="102" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B102" t="s">
         <v>26</v>
       </c>
-      <c r="C99">
-        <v>0</v>
-      </c>
-      <c r="D99">
+      <c r="C102">
+        <v>0</v>
+      </c>
+      <c r="D102">
         <f>IF(OR(AND(Tabelle12[[#This Row],[FTR/RET]]&lt;=1, Tabelle12[[#This Row],[DET]] &lt;= 19), AND(Tabelle12[[#This Row],[FTR/RET]]&lt;= 3, Tabelle12[[#This Row],[DET]] &lt;= 5)), 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="E99">
+      <c r="E102">
         <f>IF(OR(AND(Tabelle12[[#This Row],[FTR/RET]]&lt;=1, Tabelle12[[#This Row],[DET]] &gt; 20), AND(Tabelle12[[#This Row],[FTR/RET]]&lt;=5, Tabelle12[[#This Row],[FTR/RET]]&gt;=2, Tabelle12[[#This Row],[DET]] &gt;= 6, Tabelle12[[#This Row],[DET]] &lt;= 19), AND(Tabelle12[[#This Row],[FTR/RET]] &gt;= 5, Tabelle12[[#This Row],[DET]] &lt;= 5 )), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="F99">
+      <c r="F102">
         <f>IF(AND(Tabelle12[[#This Row],[Simple]]=0,Tabelle12[[#This Row],[Average]]=0), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="G99">
-        <v>0</v>
-      </c>
-      <c r="H99">
-        <v>0</v>
-      </c>
-      <c r="I99">
+      <c r="G102">
+        <v>0</v>
+      </c>
+      <c r="H102">
+        <v>0</v>
+      </c>
+      <c r="I102">
         <f>Tabelle12[[#This Row],[Count]]*(3*Tabelle12[[#This Row],[Simple]]+4*Tabelle12[[#This Row],[Average]]+6*Tabelle12[[#This Row],[Complex]])</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="100" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B100" t="s">
+      <c r="K102">
+        <f>SetTagsFP/Tabelle15[Velocity]</f>
+        <v>2.7865013774104681</v>
+      </c>
+    </row>
+    <row r="103" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B103" t="s">
         <v>27</v>
       </c>
-      <c r="C100">
+      <c r="C103">
         <v>2</v>
       </c>
-      <c r="D100">
+      <c r="D103">
         <f>IF(OR(AND(Tabelle12[[#This Row],[FTR/RET]]&lt;2, Tabelle12[[#This Row],[DET]] &lt;= 50), AND(Tabelle12[[#This Row],[FTR/RET]]&lt;=5, Tabelle12[[#This Row],[DET]] &lt; 20)), 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="E100">
+      <c r="E103">
         <f>IF(OR(AND(Tabelle12[[#This Row],[FTR/RET]]=1, Tabelle12[[#This Row],[DET]] &gt; 50), AND(Tabelle12[[#This Row],[FTR/RET]]&lt;=5, Tabelle12[[#This Row],[FTR/RET]]&gt;=2, Tabelle12[[#This Row],[DET]] &gt;= 20, Tabelle12[[#This Row],[DET]] &lt;= 50), AND(Tabelle12[[#This Row],[FTR/RET]] &gt;= 5, Tabelle12[[#This Row],[DET]] &lt; 20)), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="F100">
+      <c r="F103">
         <f>IF(AND(Tabelle12[[#This Row],[Simple]]=0,Tabelle12[[#This Row],[Average]]=0), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="G100">
-        <v>0</v>
-      </c>
-      <c r="H100">
-        <v>0</v>
-      </c>
-      <c r="I100">
+      <c r="G103">
+        <v>0</v>
+      </c>
+      <c r="H103">
+        <v>0</v>
+      </c>
+      <c r="I103">
         <f>Tabelle12[[#This Row],[Count]]*(7*Tabelle12[[#This Row],[Simple]]+10*Tabelle12[[#This Row],[Average]]+15*Tabelle12[[#This Row],[Complex]])</f>
         <v>14</v>
       </c>
-      <c r="J100" t="s">
+      <c r="J103" t="s">
         <v>59</v>
-      </c>
-    </row>
-    <row r="101" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B101" t="s">
-        <v>28</v>
-      </c>
-      <c r="C101">
-        <v>0</v>
-      </c>
-      <c r="D101">
-        <f>IF(OR(AND(Tabelle12[[#This Row],[FTR/RET]]&lt;2, Tabelle12[[#This Row],[DET]] &lt;= 50), AND(Tabelle12[[#This Row],[FTR/RET]]&lt;=5, Tabelle12[[#This Row],[DET]] &lt; 20)), 1, 0)</f>
-        <v>1</v>
-      </c>
-      <c r="E101">
-        <f>IF(OR(AND(Tabelle12[[#This Row],[FTR/RET]]=1, Tabelle12[[#This Row],[DET]] &gt; 50), AND(Tabelle12[[#This Row],[FTR/RET]]&lt;=5, Tabelle12[[#This Row],[FTR/RET]]&gt;=2, Tabelle12[[#This Row],[DET]] &gt;= 20, Tabelle12[[#This Row],[DET]] &lt;= 50), AND(Tabelle12[[#This Row],[FTR/RET]] &gt;= 5, Tabelle12[[#This Row],[DET]] &lt; 20)), 1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="F101">
-        <f>IF(AND(Tabelle12[[#This Row],[Simple]]=0,Tabelle12[[#This Row],[Average]]=0), 1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="G101">
-        <v>0</v>
-      </c>
-      <c r="H101">
-        <v>0</v>
-      </c>
-      <c r="I101">
-        <f>Tabelle12[[#This Row],[Count]]*(5*Tabelle12[[#This Row],[Simple]]+7*Tabelle12[[#This Row],[Average]]+10*Tabelle12[[#This Row],[Complex]])</f>
-        <v>0</v>
       </c>
     </row>
     <row r="104" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
+        <v>28</v>
+      </c>
+      <c r="C104">
+        <v>0</v>
+      </c>
+      <c r="D104">
+        <f>IF(OR(AND(Tabelle12[[#This Row],[FTR/RET]]&lt;2, Tabelle12[[#This Row],[DET]] &lt;= 50), AND(Tabelle12[[#This Row],[FTR/RET]]&lt;=5, Tabelle12[[#This Row],[DET]] &lt; 20)), 1, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="E104">
+        <f>IF(OR(AND(Tabelle12[[#This Row],[FTR/RET]]=1, Tabelle12[[#This Row],[DET]] &gt; 50), AND(Tabelle12[[#This Row],[FTR/RET]]&lt;=5, Tabelle12[[#This Row],[FTR/RET]]&gt;=2, Tabelle12[[#This Row],[DET]] &gt;= 20, Tabelle12[[#This Row],[DET]] &lt;= 50), AND(Tabelle12[[#This Row],[FTR/RET]] &gt;= 5, Tabelle12[[#This Row],[DET]] &lt; 20)), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="F104">
+        <f>IF(AND(Tabelle12[[#This Row],[Simple]]=0,Tabelle12[[#This Row],[Average]]=0), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="G104">
+        <v>0</v>
+      </c>
+      <c r="H104">
+        <v>0</v>
+      </c>
+      <c r="I104">
+        <f>Tabelle12[[#This Row],[Count]]*(5*Tabelle12[[#This Row],[Simple]]+7*Tabelle12[[#This Row],[Average]]+10*Tabelle12[[#This Row],[Complex]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B107" t="s">
         <v>47</v>
       </c>
-      <c r="C104" t="s">
+      <c r="C107" t="s">
         <v>21</v>
       </c>
-      <c r="D104" t="s">
+      <c r="D107" t="s">
         <v>18</v>
       </c>
-      <c r="E104" t="s">
+      <c r="E107" t="s">
         <v>19</v>
       </c>
-      <c r="F104" t="s">
+      <c r="F107" t="s">
         <v>20</v>
       </c>
-      <c r="G104" t="s">
+      <c r="G107" t="s">
         <v>49</v>
       </c>
-      <c r="H104" t="s">
+      <c r="H107" t="s">
         <v>29</v>
       </c>
-      <c r="I104" t="s">
+      <c r="I107" t="s">
         <v>50</v>
       </c>
-      <c r="J104" t="s">
+      <c r="J107" t="s">
         <v>22</v>
       </c>
-      <c r="K104" t="s">
+      <c r="K107" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="105" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B105" t="s">
+    <row r="108" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B108" t="s">
         <v>24</v>
       </c>
-      <c r="C105">
+      <c r="C108">
         <v>4</v>
       </c>
-      <c r="D105">
+      <c r="D108">
         <f>IF(OR(AND(Tabelle1214[[#This Row],[FTR/RET]]&lt;=1, Tabelle1214[[#This Row],[DET]] &lt;= 15), AND(Tabelle1214[[#This Row],[FTR/RET]]&lt;= 3, Tabelle1214[[#This Row],[DET]] &lt;= 4)), 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="E105">
+      <c r="E108">
         <f>IF(OR(AND(Tabelle1214[[#This Row],[FTR/RET]]&lt;=1, Tabelle1214[[#This Row],[DET]] &gt; 15), AND(Tabelle1214[[#This Row],[FTR/RET]]&lt;=5, Tabelle1214[[#This Row],[FTR/RET]]&gt;=2, Tabelle1214[[#This Row],[DET]] &gt;= 5, Tabelle1214[[#This Row],[DET]] &lt;= 15), AND(Tabelle1214[[#This Row],[FTR/RET]] &gt;= 5, Tabelle1214[[#This Row],[DET]] &lt;= 4 )), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="F105">
+      <c r="F108">
         <f>IF(AND(Tabelle1214[[#This Row],[Simple]]=0,Tabelle1214[[#This Row],[Average]]=0), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="G105">
-        <v>0</v>
-      </c>
-      <c r="H105">
+      <c r="G108">
+        <v>0</v>
+      </c>
+      <c r="H108">
         <v>4</v>
       </c>
-      <c r="I105">
+      <c r="I108">
         <f>Tabelle1214[[#This Row],[Count]]*(3*Tabelle1214[[#This Row],[Simple]]+4*Tabelle1214[[#This Row],[Average]]+6*Tabelle1214[[#This Row],[Complex]])</f>
         <v>12</v>
       </c>
-      <c r="J105" t="s">
+      <c r="J108" t="s">
         <v>48</v>
       </c>
-      <c r="K105">
+      <c r="K108">
         <f>SUM(Tabelle1214[Points])*0.65</f>
         <v>16.900000000000002</v>
       </c>
     </row>
-    <row r="106" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B106" t="s">
+    <row r="109" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B109" t="s">
         <v>25</v>
       </c>
-      <c r="C106">
-        <v>0</v>
-      </c>
-      <c r="D106">
+      <c r="C109">
+        <v>0</v>
+      </c>
+      <c r="D109">
         <f>IF(OR(AND(Tabelle1214[[#This Row],[FTR/RET]]&lt;=1, Tabelle1214[[#This Row],[DET]] &lt;= 19), AND(Tabelle1214[[#This Row],[FTR/RET]]&lt;= 3, Tabelle1214[[#This Row],[DET]] &lt;= 5)), 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="E106">
+      <c r="E109">
         <f>IF(OR(AND(Tabelle1214[[#This Row],[FTR/RET]]&lt;=1, Tabelle1214[[#This Row],[DET]] &gt; 20), AND(Tabelle1214[[#This Row],[FTR/RET]]&lt;=5, Tabelle1214[[#This Row],[FTR/RET]]&gt;=2, Tabelle1214[[#This Row],[DET]] &gt;= 6, Tabelle1214[[#This Row],[DET]] &lt;= 19), AND(Tabelle1214[[#This Row],[FTR/RET]] &gt;= 5, Tabelle1214[[#This Row],[DET]] &lt;= 5 )), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="F106">
+      <c r="F109">
         <f>IF(AND(Tabelle1214[[#This Row],[Simple]]=0,Tabelle1214[[#This Row],[Average]]=0), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="G106">
-        <v>0</v>
-      </c>
-      <c r="H106">
-        <v>0</v>
-      </c>
-      <c r="I106">
+      <c r="G109">
+        <v>0</v>
+      </c>
+      <c r="H109">
+        <v>0</v>
+      </c>
+      <c r="I109">
         <f>Tabelle1214[[#This Row],[Count]]*(Tabelle1214[[#This Row],[Simple]]*4+Tabelle1214[[#This Row],[Average]]*5+Tabelle1214[[#This Row],[Complex]]*7)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B107" t="s">
+    <row r="110" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B110" t="s">
         <v>26</v>
       </c>
-      <c r="C107">
-        <v>0</v>
-      </c>
-      <c r="D107">
+      <c r="C110">
+        <v>0</v>
+      </c>
+      <c r="D110">
         <f>IF(OR(AND(Tabelle1214[[#This Row],[FTR/RET]]&lt;=1, Tabelle1214[[#This Row],[DET]] &lt;= 19), AND(Tabelle1214[[#This Row],[FTR/RET]]&lt;= 3, Tabelle1214[[#This Row],[DET]] &lt;= 5)), 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="E107">
+      <c r="E110">
         <f>IF(OR(AND(Tabelle1214[[#This Row],[FTR/RET]]&lt;=1, Tabelle1214[[#This Row],[DET]] &gt; 20), AND(Tabelle1214[[#This Row],[FTR/RET]]&lt;=5, Tabelle1214[[#This Row],[FTR/RET]]&gt;=2, Tabelle1214[[#This Row],[DET]] &gt;= 6, Tabelle1214[[#This Row],[DET]] &lt;= 19), AND(Tabelle1214[[#This Row],[FTR/RET]] &gt;= 5, Tabelle1214[[#This Row],[DET]] &lt;= 5 )), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="F107">
+      <c r="F110">
         <f>IF(AND(Tabelle1214[[#This Row],[Simple]]=0,Tabelle1214[[#This Row],[Average]]=0), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="G107">
-        <v>0</v>
-      </c>
-      <c r="H107">
-        <v>0</v>
-      </c>
-      <c r="I107">
+      <c r="G110">
+        <v>0</v>
+      </c>
+      <c r="H110">
+        <v>0</v>
+      </c>
+      <c r="I110">
         <f>Tabelle1214[[#This Row],[Count]]*(3*Tabelle1214[[#This Row],[Simple]]+4*Tabelle1214[[#This Row],[Average]]+6*Tabelle1214[[#This Row],[Complex]])</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="108" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B108" t="s">
+      <c r="K110">
+        <f>AdministrateBarsFP/Tabelle15[Velocity]</f>
+        <v>4.2617079889807163</v>
+      </c>
+    </row>
+    <row r="111" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B111" t="s">
         <v>27</v>
       </c>
-      <c r="C108">
+      <c r="C111">
         <v>2</v>
       </c>
-      <c r="D108">
+      <c r="D111">
         <f>IF(OR(AND(Tabelle1214[[#This Row],[FTR/RET]]&lt;2, Tabelle1214[[#This Row],[DET]] &lt;= 50), AND(Tabelle1214[[#This Row],[FTR/RET]]&lt;=5, Tabelle1214[[#This Row],[DET]] &lt; 20)), 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="E108">
+      <c r="E111">
         <f>IF(OR(AND(Tabelle1214[[#This Row],[FTR/RET]]=1, Tabelle1214[[#This Row],[DET]] &gt; 50), AND(Tabelle1214[[#This Row],[FTR/RET]]&lt;=5, Tabelle1214[[#This Row],[FTR/RET]]&gt;=2, Tabelle1214[[#This Row],[DET]] &gt;= 20, Tabelle1214[[#This Row],[DET]] &lt;= 50), AND(Tabelle1214[[#This Row],[FTR/RET]] &gt;= 5, Tabelle1214[[#This Row],[DET]] &lt; 20)), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="F108">
+      <c r="F111">
         <f>IF(AND(Tabelle1214[[#This Row],[Simple]]=0,Tabelle1214[[#This Row],[Average]]=0), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="G108">
-        <v>0</v>
-      </c>
-      <c r="H108">
-        <v>0</v>
-      </c>
-      <c r="I108">
+      <c r="G111">
+        <v>0</v>
+      </c>
+      <c r="H111">
+        <v>0</v>
+      </c>
+      <c r="I111">
         <f>Tabelle1214[[#This Row],[Count]]*(7*Tabelle1214[[#This Row],[Simple]]+10*Tabelle1214[[#This Row],[Average]]+15*Tabelle1214[[#This Row],[Complex]])</f>
         <v>14</v>
       </c>
-      <c r="J108" t="s">
+      <c r="J111" t="s">
         <v>60</v>
-      </c>
-    </row>
-    <row r="109" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B109" t="s">
-        <v>28</v>
-      </c>
-      <c r="C109">
-        <v>0</v>
-      </c>
-      <c r="D109">
-        <f>IF(OR(AND(Tabelle1214[[#This Row],[FTR/RET]]&lt;2, Tabelle1214[[#This Row],[DET]] &lt;= 50), AND(Tabelle1214[[#This Row],[FTR/RET]]&lt;=5, Tabelle1214[[#This Row],[DET]] &lt; 20)), 1, 0)</f>
-        <v>1</v>
-      </c>
-      <c r="E109">
-        <f>IF(OR(AND(Tabelle1214[[#This Row],[FTR/RET]]=1, Tabelle1214[[#This Row],[DET]] &gt; 50), AND(Tabelle1214[[#This Row],[FTR/RET]]&lt;=5, Tabelle1214[[#This Row],[FTR/RET]]&gt;=2, Tabelle1214[[#This Row],[DET]] &gt;= 20, Tabelle1214[[#This Row],[DET]] &lt;= 50), AND(Tabelle1214[[#This Row],[FTR/RET]] &gt;= 5, Tabelle1214[[#This Row],[DET]] &lt; 20)), 1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="F109">
-        <f>IF(AND(Tabelle1214[[#This Row],[Simple]]=0,Tabelle1214[[#This Row],[Average]]=0), 1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="G109">
-        <v>0</v>
-      </c>
-      <c r="H109">
-        <v>0</v>
-      </c>
-      <c r="I109">
-        <f>Tabelle1214[[#This Row],[Count]]*(5*Tabelle1214[[#This Row],[Simple]]+7*Tabelle1214[[#This Row],[Average]]+10*Tabelle1214[[#This Row],[Complex]])</f>
-        <v>0</v>
       </c>
     </row>
     <row r="112" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
-        <v>32</v>
-      </c>
-      <c r="C112" t="s">
-        <v>21</v>
-      </c>
-      <c r="D112" t="s">
-        <v>18</v>
-      </c>
-      <c r="E112" t="s">
-        <v>19</v>
-      </c>
-      <c r="F112" t="s">
-        <v>20</v>
-      </c>
-      <c r="G112" t="s">
-        <v>49</v>
-      </c>
-      <c r="H112" t="s">
-        <v>29</v>
-      </c>
-      <c r="I112" t="s">
-        <v>50</v>
-      </c>
-      <c r="J112" t="s">
-        <v>22</v>
-      </c>
-      <c r="K112" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="113" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B113" t="s">
-        <v>24</v>
-      </c>
-      <c r="C113">
-        <v>0</v>
-      </c>
-      <c r="D113">
-        <f>IF(OR(AND(Tabelle121415[[#This Row],[FTR/RET]]&lt;=1, Tabelle121415[[#This Row],[DET]] &lt;= 15), AND(Tabelle121415[[#This Row],[FTR/RET]]&lt;= 3, Tabelle121415[[#This Row],[DET]] &lt;= 4)), 1, 0)</f>
-        <v>1</v>
-      </c>
-      <c r="E113">
-        <f>IF(OR(AND(Tabelle121415[[#This Row],[FTR/RET]]&lt;=1, Tabelle121415[[#This Row],[DET]] &gt; 15), AND(Tabelle121415[[#This Row],[FTR/RET]]&lt;=5, Tabelle121415[[#This Row],[FTR/RET]]&gt;=2, Tabelle121415[[#This Row],[DET]] &gt;= 5, Tabelle121415[[#This Row],[DET]] &lt;= 15), AND(Tabelle121415[[#This Row],[FTR/RET]] &gt;= 5, Tabelle121415[[#This Row],[DET]] &lt;= 4 )), 1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="F113">
-        <f>IF(AND(Tabelle121415[[#This Row],[Simple]]=0,Tabelle121415[[#This Row],[Average]]=0), 1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="G113">
-        <v>0</v>
-      </c>
-      <c r="H113">
-        <v>0</v>
-      </c>
-      <c r="I113">
-        <f>Tabelle121415[[#This Row],[Count]]*(3*Tabelle121415[[#This Row],[Simple]]+4*Tabelle121415[[#This Row],[Average]]+6*Tabelle121415[[#This Row],[Complex]])</f>
-        <v>0</v>
-      </c>
-      <c r="K113">
-        <f>SUM(Tabelle121415[Points])*0.65</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="114" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B114" t="s">
-        <v>25</v>
-      </c>
-      <c r="C114">
-        <v>0</v>
-      </c>
-      <c r="D114">
-        <f>IF(OR(AND(Tabelle121415[[#This Row],[FTR/RET]]&lt;=1, Tabelle121415[[#This Row],[DET]] &lt;= 19), AND(Tabelle121415[[#This Row],[FTR/RET]]&lt;= 3, Tabelle121415[[#This Row],[DET]] &lt;= 5)), 1, 0)</f>
-        <v>1</v>
-      </c>
-      <c r="E114">
-        <f>IF(OR(AND(Tabelle121415[[#This Row],[FTR/RET]]&lt;=1, Tabelle121415[[#This Row],[DET]] &gt; 20), AND(Tabelle121415[[#This Row],[FTR/RET]]&lt;=5, Tabelle121415[[#This Row],[FTR/RET]]&gt;=2, Tabelle121415[[#This Row],[DET]] &gt;= 6, Tabelle121415[[#This Row],[DET]] &lt;= 19), AND(Tabelle121415[[#This Row],[FTR/RET]] &gt;= 5, Tabelle121415[[#This Row],[DET]] &lt;= 5 )), 1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="F114">
-        <f>IF(AND(Tabelle121415[[#This Row],[Simple]]=0,Tabelle121415[[#This Row],[Average]]=0), 1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="G114">
-        <v>0</v>
-      </c>
-      <c r="H114">
-        <v>0</v>
-      </c>
-      <c r="I114">
-        <f>Tabelle121415[[#This Row],[Count]]*(Tabelle121415[[#This Row],[Simple]]*4+Tabelle121415[[#This Row],[Average]]*5+Tabelle121415[[#This Row],[Complex]]*7)</f>
+        <v>28</v>
+      </c>
+      <c r="C112">
+        <v>0</v>
+      </c>
+      <c r="D112">
+        <f>IF(OR(AND(Tabelle1214[[#This Row],[FTR/RET]]&lt;2, Tabelle1214[[#This Row],[DET]] &lt;= 50), AND(Tabelle1214[[#This Row],[FTR/RET]]&lt;=5, Tabelle1214[[#This Row],[DET]] &lt; 20)), 1, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="E112">
+        <f>IF(OR(AND(Tabelle1214[[#This Row],[FTR/RET]]=1, Tabelle1214[[#This Row],[DET]] &gt; 50), AND(Tabelle1214[[#This Row],[FTR/RET]]&lt;=5, Tabelle1214[[#This Row],[FTR/RET]]&gt;=2, Tabelle1214[[#This Row],[DET]] &gt;= 20, Tabelle1214[[#This Row],[DET]] &lt;= 50), AND(Tabelle1214[[#This Row],[FTR/RET]] &gt;= 5, Tabelle1214[[#This Row],[DET]] &lt; 20)), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="F112">
+        <f>IF(AND(Tabelle1214[[#This Row],[Simple]]=0,Tabelle1214[[#This Row],[Average]]=0), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="G112">
+        <v>0</v>
+      </c>
+      <c r="H112">
+        <v>0</v>
+      </c>
+      <c r="I112">
+        <f>Tabelle1214[[#This Row],[Count]]*(5*Tabelle1214[[#This Row],[Simple]]+7*Tabelle1214[[#This Row],[Average]]+10*Tabelle1214[[#This Row],[Complex]])</f>
         <v>0</v>
       </c>
     </row>
     <row r="115" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
-        <v>26</v>
-      </c>
-      <c r="C115">
-        <v>0</v>
-      </c>
-      <c r="D115">
-        <f>IF(OR(AND(Tabelle121415[[#This Row],[FTR/RET]]&lt;=1, Tabelle121415[[#This Row],[DET]] &lt;= 19), AND(Tabelle121415[[#This Row],[FTR/RET]]&lt;= 3, Tabelle121415[[#This Row],[DET]] &lt;= 5)), 1, 0)</f>
-        <v>1</v>
-      </c>
-      <c r="E115">
-        <f>IF(OR(AND(Tabelle121415[[#This Row],[FTR/RET]]&lt;=1, Tabelle121415[[#This Row],[DET]] &gt; 20), AND(Tabelle121415[[#This Row],[FTR/RET]]&lt;=5, Tabelle121415[[#This Row],[FTR/RET]]&gt;=2, Tabelle121415[[#This Row],[DET]] &gt;= 6, Tabelle121415[[#This Row],[DET]] &lt;= 19), AND(Tabelle121415[[#This Row],[FTR/RET]] &gt;= 5, Tabelle121415[[#This Row],[DET]] &lt;= 5 )), 1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="F115">
-        <f>IF(AND(Tabelle121415[[#This Row],[Simple]]=0,Tabelle121415[[#This Row],[Average]]=0), 1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="G115">
-        <v>0</v>
-      </c>
-      <c r="H115">
-        <v>0</v>
-      </c>
-      <c r="I115">
-        <f>Tabelle121415[[#This Row],[Count]]*(3*Tabelle121415[[#This Row],[Simple]]+4*Tabelle121415[[#This Row],[Average]]+6*Tabelle121415[[#This Row],[Complex]])</f>
-        <v>0</v>
+        <v>32</v>
+      </c>
+      <c r="C115" t="s">
+        <v>21</v>
+      </c>
+      <c r="D115" t="s">
+        <v>18</v>
+      </c>
+      <c r="E115" t="s">
+        <v>19</v>
+      </c>
+      <c r="F115" t="s">
+        <v>20</v>
+      </c>
+      <c r="G115" t="s">
+        <v>49</v>
+      </c>
+      <c r="H115" t="s">
+        <v>29</v>
+      </c>
+      <c r="I115" t="s">
+        <v>50</v>
+      </c>
+      <c r="J115" t="s">
+        <v>22</v>
+      </c>
+      <c r="K115" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="116" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C116">
         <v>0</v>
       </c>
       <c r="D116">
-        <f>IF(OR(AND(Tabelle121415[[#This Row],[FTR/RET]]&lt;2, Tabelle121415[[#This Row],[DET]] &lt;= 50), AND(Tabelle121415[[#This Row],[FTR/RET]]&lt;=5, Tabelle121415[[#This Row],[DET]] &lt; 20)), 1, 0)</f>
+        <f>IF(OR(AND(Tabelle121415[[#This Row],[FTR/RET]]&lt;=1, Tabelle121415[[#This Row],[DET]] &lt;= 15), AND(Tabelle121415[[#This Row],[FTR/RET]]&lt;= 3, Tabelle121415[[#This Row],[DET]] &lt;= 4)), 1, 0)</f>
         <v>1</v>
       </c>
       <c r="E116">
-        <f>IF(OR(AND(Tabelle121415[[#This Row],[FTR/RET]]=1, Tabelle121415[[#This Row],[DET]] &gt; 50), AND(Tabelle121415[[#This Row],[FTR/RET]]&lt;=5, Tabelle121415[[#This Row],[FTR/RET]]&gt;=2, Tabelle121415[[#This Row],[DET]] &gt;= 20, Tabelle121415[[#This Row],[DET]] &lt;= 50), AND(Tabelle121415[[#This Row],[FTR/RET]] &gt;= 5, Tabelle121415[[#This Row],[DET]] &lt; 20)), 1, 0)</f>
+        <f>IF(OR(AND(Tabelle121415[[#This Row],[FTR/RET]]&lt;=1, Tabelle121415[[#This Row],[DET]] &gt; 15), AND(Tabelle121415[[#This Row],[FTR/RET]]&lt;=5, Tabelle121415[[#This Row],[FTR/RET]]&gt;=2, Tabelle121415[[#This Row],[DET]] &gt;= 5, Tabelle121415[[#This Row],[DET]] &lt;= 15), AND(Tabelle121415[[#This Row],[FTR/RET]] &gt;= 5, Tabelle121415[[#This Row],[DET]] &lt;= 4 )), 1, 0)</f>
         <v>0</v>
       </c>
       <c r="F116">
@@ -4175,23 +4350,27 @@
         <v>0</v>
       </c>
       <c r="I116">
-        <f>Tabelle121415[[#This Row],[Count]]*(7*Tabelle121415[[#This Row],[Simple]]+10*Tabelle121415[[#This Row],[Average]]+15*Tabelle121415[[#This Row],[Complex]])</f>
+        <f>Tabelle121415[[#This Row],[Count]]*(3*Tabelle121415[[#This Row],[Simple]]+4*Tabelle121415[[#This Row],[Average]]+6*Tabelle121415[[#This Row],[Complex]])</f>
+        <v>0</v>
+      </c>
+      <c r="K116">
+        <f>SUM(Tabelle121415[Points])*0.65</f>
         <v>0</v>
       </c>
     </row>
     <row r="117" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B117" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C117">
         <v>0</v>
       </c>
       <c r="D117">
-        <f>IF(OR(AND(Tabelle121415[[#This Row],[FTR/RET]]&lt;2, Tabelle121415[[#This Row],[DET]] &lt;= 50), AND(Tabelle121415[[#This Row],[FTR/RET]]&lt;=5, Tabelle121415[[#This Row],[DET]] &lt; 20)), 1, 0)</f>
+        <f>IF(OR(AND(Tabelle121415[[#This Row],[FTR/RET]]&lt;=1, Tabelle121415[[#This Row],[DET]] &lt;= 19), AND(Tabelle121415[[#This Row],[FTR/RET]]&lt;= 3, Tabelle121415[[#This Row],[DET]] &lt;= 5)), 1, 0)</f>
         <v>1</v>
       </c>
       <c r="E117">
-        <f>IF(OR(AND(Tabelle121415[[#This Row],[FTR/RET]]=1, Tabelle121415[[#This Row],[DET]] &gt; 50), AND(Tabelle121415[[#This Row],[FTR/RET]]&lt;=5, Tabelle121415[[#This Row],[FTR/RET]]&gt;=2, Tabelle121415[[#This Row],[DET]] &gt;= 20, Tabelle121415[[#This Row],[DET]] &lt;= 50), AND(Tabelle121415[[#This Row],[FTR/RET]] &gt;= 5, Tabelle121415[[#This Row],[DET]] &lt; 20)), 1, 0)</f>
+        <f>IF(OR(AND(Tabelle121415[[#This Row],[FTR/RET]]&lt;=1, Tabelle121415[[#This Row],[DET]] &gt; 20), AND(Tabelle121415[[#This Row],[FTR/RET]]&lt;=5, Tabelle121415[[#This Row],[FTR/RET]]&gt;=2, Tabelle121415[[#This Row],[DET]] &gt;= 6, Tabelle121415[[#This Row],[DET]] &lt;= 19), AND(Tabelle121415[[#This Row],[FTR/RET]] &gt;= 5, Tabelle121415[[#This Row],[DET]] &lt;= 5 )), 1, 0)</f>
         <v>0</v>
       </c>
       <c r="F117">
@@ -4205,6 +4384,96 @@
         <v>0</v>
       </c>
       <c r="I117">
+        <f>Tabelle121415[[#This Row],[Count]]*(Tabelle121415[[#This Row],[Simple]]*4+Tabelle121415[[#This Row],[Average]]*5+Tabelle121415[[#This Row],[Complex]]*7)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B118" t="s">
+        <v>26</v>
+      </c>
+      <c r="C118">
+        <v>0</v>
+      </c>
+      <c r="D118">
+        <f>IF(OR(AND(Tabelle121415[[#This Row],[FTR/RET]]&lt;=1, Tabelle121415[[#This Row],[DET]] &lt;= 19), AND(Tabelle121415[[#This Row],[FTR/RET]]&lt;= 3, Tabelle121415[[#This Row],[DET]] &lt;= 5)), 1, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="E118">
+        <f>IF(OR(AND(Tabelle121415[[#This Row],[FTR/RET]]&lt;=1, Tabelle121415[[#This Row],[DET]] &gt; 20), AND(Tabelle121415[[#This Row],[FTR/RET]]&lt;=5, Tabelle121415[[#This Row],[FTR/RET]]&gt;=2, Tabelle121415[[#This Row],[DET]] &gt;= 6, Tabelle121415[[#This Row],[DET]] &lt;= 19), AND(Tabelle121415[[#This Row],[FTR/RET]] &gt;= 5, Tabelle121415[[#This Row],[DET]] &lt;= 5 )), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="F118">
+        <f>IF(AND(Tabelle121415[[#This Row],[Simple]]=0,Tabelle121415[[#This Row],[Average]]=0), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="G118">
+        <v>0</v>
+      </c>
+      <c r="H118">
+        <v>0</v>
+      </c>
+      <c r="I118">
+        <f>Tabelle121415[[#This Row],[Count]]*(3*Tabelle121415[[#This Row],[Simple]]+4*Tabelle121415[[#This Row],[Average]]+6*Tabelle121415[[#This Row],[Complex]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B119" t="s">
+        <v>27</v>
+      </c>
+      <c r="C119">
+        <v>0</v>
+      </c>
+      <c r="D119">
+        <f>IF(OR(AND(Tabelle121415[[#This Row],[FTR/RET]]&lt;2, Tabelle121415[[#This Row],[DET]] &lt;= 50), AND(Tabelle121415[[#This Row],[FTR/RET]]&lt;=5, Tabelle121415[[#This Row],[DET]] &lt; 20)), 1, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="E119">
+        <f>IF(OR(AND(Tabelle121415[[#This Row],[FTR/RET]]=1, Tabelle121415[[#This Row],[DET]] &gt; 50), AND(Tabelle121415[[#This Row],[FTR/RET]]&lt;=5, Tabelle121415[[#This Row],[FTR/RET]]&gt;=2, Tabelle121415[[#This Row],[DET]] &gt;= 20, Tabelle121415[[#This Row],[DET]] &lt;= 50), AND(Tabelle121415[[#This Row],[FTR/RET]] &gt;= 5, Tabelle121415[[#This Row],[DET]] &lt; 20)), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="F119">
+        <f>IF(AND(Tabelle121415[[#This Row],[Simple]]=0,Tabelle121415[[#This Row],[Average]]=0), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="G119">
+        <v>0</v>
+      </c>
+      <c r="H119">
+        <v>0</v>
+      </c>
+      <c r="I119">
+        <f>Tabelle121415[[#This Row],[Count]]*(7*Tabelle121415[[#This Row],[Simple]]+10*Tabelle121415[[#This Row],[Average]]+15*Tabelle121415[[#This Row],[Complex]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B120" t="s">
+        <v>28</v>
+      </c>
+      <c r="C120">
+        <v>0</v>
+      </c>
+      <c r="D120">
+        <f>IF(OR(AND(Tabelle121415[[#This Row],[FTR/RET]]&lt;2, Tabelle121415[[#This Row],[DET]] &lt;= 50), AND(Tabelle121415[[#This Row],[FTR/RET]]&lt;=5, Tabelle121415[[#This Row],[DET]] &lt; 20)), 1, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="E120">
+        <f>IF(OR(AND(Tabelle121415[[#This Row],[FTR/RET]]=1, Tabelle121415[[#This Row],[DET]] &gt; 50), AND(Tabelle121415[[#This Row],[FTR/RET]]&lt;=5, Tabelle121415[[#This Row],[FTR/RET]]&gt;=2, Tabelle121415[[#This Row],[DET]] &gt;= 20, Tabelle121415[[#This Row],[DET]] &lt;= 50), AND(Tabelle121415[[#This Row],[FTR/RET]] &gt;= 5, Tabelle121415[[#This Row],[DET]] &lt; 20)), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="F120">
+        <f>IF(AND(Tabelle121415[[#This Row],[Simple]]=0,Tabelle121415[[#This Row],[Average]]=0), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="G120">
+        <v>0</v>
+      </c>
+      <c r="H120">
+        <v>0</v>
+      </c>
+      <c r="I120">
         <f>Tabelle121415[[#This Row],[Count]]*(5*Tabelle121415[[#This Row],[Simple]]+7*Tabelle121415[[#This Row],[Average]]+10*Tabelle121415[[#This Row],[Complex]])</f>
         <v>0</v>
       </c>
@@ -4213,7 +4482,7 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
-  <tableParts count="14">
+  <tableParts count="15">
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
@@ -4228,6 +4497,7 @@
     <tablePart r:id="rId14"/>
     <tablePart r:id="rId15"/>
     <tablePart r:id="rId16"/>
+    <tablePart r:id="rId17"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated times spent document based on JIRA times
</commit_message>
<xml_diff>
--- a/TimesSpent.xlsx
+++ b/TimesSpent.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phili\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phili\Documents\GitHub\KaNiBa\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="69">
   <si>
     <t>UC Name</t>
   </si>
@@ -242,6 +242,9 @@
   </si>
   <si>
     <t>Estimate</t>
+  </si>
+  <si>
+    <t>The UI was very different hand had to be reworked serveral times to serve function as expected</t>
   </si>
 </sst>
 </file>
@@ -292,6 +295,18 @@
   </cellStyles>
   <dxfs count="10">
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     </dxf>
     <dxf>
@@ -308,18 +323,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="25" formatCode="hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -536,13 +539,13 @@
                   <c:v>0.27083333333333331</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>0.29166666666666663</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>8.9583333333333334E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>0.19444444444444442</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -557,11 +560,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="309151616"/>
-        <c:axId val="309155144"/>
+        <c:axId val="214389000"/>
+        <c:axId val="214388608"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="309151616"/>
+        <c:axId val="214389000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -618,12 +621,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="309155144"/>
+        <c:crossAx val="214388608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="309155144"/>
+        <c:axId val="214388608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -680,7 +683,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="309151616"/>
+        <c:crossAx val="214389000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2.0833300000000003E-2"/>
@@ -833,18 +836,18 @@
   <tableColumns count="12">
     <tableColumn id="1" name="UC Name"/>
     <tableColumn id="2" name="Documentation"/>
-    <tableColumn id="7" name="UI Design" dataDxfId="5"/>
-    <tableColumn id="8" name="Database" dataDxfId="4"/>
-    <tableColumn id="9" name="Warmup Phase" dataDxfId="3"/>
+    <tableColumn id="7" name="UI Design" dataDxfId="9"/>
+    <tableColumn id="8" name="Database" dataDxfId="8"/>
+    <tableColumn id="9" name="Warmup Phase" dataDxfId="7"/>
     <tableColumn id="3" name="Coding"/>
     <tableColumn id="4" name="Testing"/>
-    <tableColumn id="10" name="Total w/o warmup" dataDxfId="2">
+    <tableColumn id="10" name="Total w/o warmup" dataDxfId="6">
       <calculatedColumnFormula>SUM(Tabelle1[[#This Row],[Documentation]:[Database]])+SUM(Tabelle1[[#This Row],[Coding]:[Testing]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Total" dataDxfId="1">
+    <tableColumn id="5" name="Total" dataDxfId="5">
       <calculatedColumnFormula>SUM(Tabelle1[[#This Row],[Documentation]:[Testing]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Estimate" dataDxfId="0">
+    <tableColumn id="12" name="Estimate" dataDxfId="4">
       <calculatedColumnFormula>Tabelle1[[#This Row],[FP]]/Tabelle15[Velocity]/24</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" name="FP"/>
@@ -963,13 +966,13 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Tabelle15" displayName="Tabelle15" ref="O23:Q24" totalsRowShown="0">
   <autoFilter ref="O23:Q24"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Time spent (w/o outliers)" dataDxfId="7">
-      <calculatedColumnFormula>SUM(I3:I10,I12)*24</calculatedColumnFormula>
+    <tableColumn id="1" name="Time spent (w/o outliers)" dataDxfId="1">
+      <calculatedColumnFormula>SUM(I3:I10,I12,I14:I15)*24</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" name="Function Points (w/o outliers)">
-      <calculatedColumnFormula>SUM(L3:L10,L12)</calculatedColumnFormula>
+      <calculatedColumnFormula>SUM(L3:L10,L12,L14:L15)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Velocity" dataDxfId="6">
+    <tableColumn id="3" name="Velocity" dataDxfId="0">
       <calculatedColumnFormula>P24/O24</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -984,10 +987,10 @@
     <tableColumn id="1" name="Search bar"/>
     <tableColumn id="2" name="Count"/>
     <tableColumn id="3" name="Simple"/>
-    <tableColumn id="4" name="Average" dataDxfId="9">
+    <tableColumn id="4" name="Average" dataDxfId="3">
       <calculatedColumnFormula>IF(OR(AND(Tabelle2[[#This Row],[FTR/RET]]=1, Tabelle2[[#This Row],[DET]] &gt; 50), AND(Tabelle2[[#This Row],[FTR/RET]]&lt;=5, Tabelle2[[#This Row],[FTR/RET]]&gt;=2, Tabelle2[[#This Row],[DET]] &gt;= 20, Tabelle2[[#This Row],[DET]] &lt;= 50), AND(Tabelle2[[#This Row],[FTR/RET]] &gt;= 5, Tabelle2[[#This Row],[DET]] &lt; 20)), "x", "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Complex" dataDxfId="8">
+    <tableColumn id="5" name="Complex" dataDxfId="2">
       <calculatedColumnFormula>IF(AND(Tabelle2[[#This Row],[Simple]]="",Tabelle2[[#This Row],[Average]]=""), "x", "")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" name="FTR/RET"/>
@@ -1413,8 +1416,8 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="B2:Q120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="Q24" sqref="Q24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1497,7 +1500,7 @@
       </c>
       <c r="K3" s="2">
         <f>Tabelle1[[#This Row],[FP]]/Tabelle15[Velocity]/24</f>
-        <v>0.11610422405876951</v>
+        <v>0.11552875243664716</v>
       </c>
       <c r="L3">
         <f>CommentFP</f>
@@ -1536,7 +1539,7 @@
       </c>
       <c r="K4" s="2">
         <f>Tabelle1[[#This Row],[FP]]/Tabelle15[Velocity]/24</f>
-        <v>0.14342286501377408</v>
+        <v>0.14271198830409354</v>
       </c>
       <c r="L4">
         <f>SeePinboardsFP</f>
@@ -1575,7 +1578,7 @@
       </c>
       <c r="K5" s="2">
         <f>Tabelle1[[#This Row],[FP]]/Tabelle15[Velocity]/24</f>
-        <v>0.16391184573002754</v>
+        <v>0.16309941520467836</v>
       </c>
       <c r="L5">
         <f>LoginFP</f>
@@ -1614,7 +1617,7 @@
       </c>
       <c r="K6" s="2">
         <f>Tabelle1[[#This Row],[FP]]/Tabelle15[Velocity]/24</f>
-        <v>0.18387546796637702</v>
+        <v>0.1829640875693507</v>
       </c>
       <c r="L6">
         <f>RateBarFP</f>
@@ -1656,7 +1659,7 @@
       </c>
       <c r="K7" s="2">
         <f>Tabelle1[[#This Row],[FP]]/Tabelle15[Velocity]/24</f>
-        <v>0.14342286501377408</v>
+        <v>0.14271198830409354</v>
       </c>
       <c r="L7">
         <f>SearchBarFP</f>
@@ -1695,7 +1698,7 @@
       </c>
       <c r="K8" s="2">
         <f>Tabelle1[[#This Row],[FP]]/Tabelle15[Velocity]/24</f>
-        <v>0.19123048668503209</v>
+        <v>0.19028265107212472</v>
       </c>
       <c r="L8">
         <f>GetBarInfoFP</f>
@@ -1734,7 +1737,7 @@
       </c>
       <c r="K9" s="2">
         <f>Tabelle1[[#This Row],[FP]]/Tabelle15[Velocity]/24</f>
-        <v>0.19858550540368722</v>
+        <v>0.19760121457489876</v>
       </c>
       <c r="L9">
         <f>SurveysFP</f>
@@ -1773,7 +1776,7 @@
       </c>
       <c r="K10" s="2">
         <f>Tabelle1[[#This Row],[FP]]/Tabelle15[Velocity]/24</f>
-        <v>0.21171946740128558</v>
+        <v>0.21067007797270954</v>
       </c>
       <c r="L10">
         <f>SeeMapsFP</f>
@@ -1812,7 +1815,7 @@
       </c>
       <c r="K11" s="2">
         <f>Tabelle1[[#This Row],[FP]]/Tabelle15[Velocity]/24</f>
-        <v>0.30050505050505044</v>
+        <v>0.29901559454191029</v>
       </c>
       <c r="L11">
         <f>ChangeInfoFP</f>
@@ -1854,7 +1857,7 @@
       </c>
       <c r="K12" s="2">
         <f>Tabelle1[[#This Row],[FP]]/Tabelle15[Velocity]/24</f>
-        <v>0.30050505050505044</v>
+        <v>0.29901559454191029</v>
       </c>
       <c r="L12">
         <f>RegisterFp</f>
@@ -1865,50 +1868,77 @@
       <c r="B13" t="s">
         <v>43</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
+      <c r="C13" s="1">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0.125</v>
+      </c>
+      <c r="E13" s="1">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="F13" s="1">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="G13" s="1">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="H13" s="1">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="I13" s="1">
         <f>SUM(Tabelle1[[#This Row],[Documentation]:[Database]])+SUM(Tabelle1[[#This Row],[Coding]:[Testing]])</f>
-        <v>0</v>
+        <v>0.29166666666666663</v>
       </c>
       <c r="J13" s="2">
         <f>SUM(Tabelle1[[#This Row],[Documentation]:[Testing]])</f>
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="K13" s="2">
         <f>Tabelle1[[#This Row],[FP]]/Tabelle15[Velocity]/24</f>
-        <v>0.21171946740128558</v>
+        <v>0.21067007797270954</v>
       </c>
       <c r="L13">
         <f>SeeMapsFP</f>
         <v>20.150000000000002</v>
       </c>
+      <c r="M13" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>45</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
+      <c r="C14" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="D14" s="1">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="E14" s="1">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0</v>
+      </c>
+      <c r="G14" s="1">
+        <v>4.4444444444444446E-2</v>
+      </c>
+      <c r="H14" s="1">
+        <v>6.9444444444444441E-3</v>
+      </c>
       <c r="I14" s="1">
         <f>SUM(Tabelle1[[#This Row],[Documentation]:[Database]])+SUM(Tabelle1[[#This Row],[Coding]:[Testing]])</f>
-        <v>0</v>
+        <v>8.9583333333333334E-2</v>
       </c>
       <c r="J14" s="2">
         <f>SUM(Tabelle1[[#This Row],[Documentation]:[Testing]])</f>
-        <v>0</v>
+        <v>8.9583333333333348E-2</v>
       </c>
       <c r="K14" s="2">
         <f>Tabelle1[[#This Row],[FP]]/Tabelle15[Velocity]/24</f>
-        <v>0.11610422405876951</v>
+        <v>0.11552875243664716</v>
       </c>
       <c r="L14">
         <f>SetTagsFP</f>
@@ -1919,23 +1949,35 @@
       <c r="B15" t="s">
         <v>47</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
+      <c r="C15" s="1">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D15" s="1">
+        <v>5.5555555555555552E-2</v>
+      </c>
+      <c r="E15" s="1">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0</v>
+      </c>
+      <c r="G15" s="1">
+        <v>9.7222222222222224E-2</v>
+      </c>
+      <c r="H15" s="1">
+        <v>6.9444444444444441E-3</v>
+      </c>
       <c r="I15" s="1">
         <f>SUM(Tabelle1[[#This Row],[Documentation]:[Database]])+SUM(Tabelle1[[#This Row],[Coding]:[Testing]])</f>
-        <v>0</v>
+        <v>0.19444444444444442</v>
       </c>
       <c r="J15" s="2">
         <f>SUM(Tabelle1[[#This Row],[Documentation]:[Testing]])</f>
-        <v>0</v>
+        <v>0.19444444444444445</v>
       </c>
       <c r="K15" s="2">
         <f>Tabelle1[[#This Row],[FP]]/Tabelle15[Velocity]/24</f>
-        <v>0.17757116620752986</v>
+        <v>0.17669103313840154</v>
       </c>
       <c r="L15">
         <f>AdministrateBarsFP</f>
@@ -2168,16 +2210,16 @@
         <v>30</v>
       </c>
       <c r="O24" s="4">
-        <f>SUM(I3:I10,I12)*24</f>
-        <v>39.666666666666664</v>
+        <f>SUM(I3:I10,I12,I14:I15)*24</f>
+        <v>46.483333333333334</v>
       </c>
       <c r="P24">
-        <f>SUM(L3:L10,L12)</f>
-        <v>157.30000000000001</v>
+        <f>SUM(L3:L10,L12,L14:L15)</f>
+        <v>185.25000000000003</v>
       </c>
       <c r="Q24" s="3">
         <f>P24/O24</f>
-        <v>3.9655462184873955</v>
+        <v>3.985299390462532</v>
       </c>
     </row>
     <row r="27" spans="2:17" x14ac:dyDescent="0.25">
@@ -3831,7 +3873,7 @@
       </c>
       <c r="K94">
         <f>SeeMapsFP/Tabelle15[Velocity]</f>
-        <v>5.0812672176308542</v>
+        <v>5.0560818713450288</v>
       </c>
     </row>
     <row r="95" spans="2:11" x14ac:dyDescent="0.25">
@@ -4030,7 +4072,7 @@
       </c>
       <c r="K102">
         <f>SetTagsFP/Tabelle15[Velocity]</f>
-        <v>2.7865013774104681</v>
+        <v>2.7726900584795318</v>
       </c>
     </row>
     <row r="103" spans="2:11" x14ac:dyDescent="0.25">
@@ -4226,7 +4268,7 @@
       </c>
       <c r="K110">
         <f>AdministrateBarsFP/Tabelle15[Velocity]</f>
-        <v>4.2617079889807163</v>
+        <v>4.2405847953216371</v>
       </c>
     </row>
     <row r="111" spans="2:11" x14ac:dyDescent="0.25">

</xml_diff>